<commit_message>
ajout script courbes dose relative
</commit_message>
<xml_diff>
--- a/RT3/mesures/RT3_absolue.xlsx
+++ b/RT3/mesures/RT3_absolue.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrerintaud/Desktop/RT/mesures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/LEXAR/Fiches_DQ/RT/RT3/mesures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AD2121-4EB8-014D-8F78-C64815F6E15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3033CC60-0074-1D42-B83C-618EA67EC80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="1" xr2:uid="{0B3496DC-FE75-484B-81FB-5E96C744887E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{0B3496DC-FE75-484B-81FB-5E96C744887E}"/>
   </bookViews>
   <sheets>
     <sheet name="Facteurs correctifs" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="78">
   <si>
     <t>X6</t>
   </si>
@@ -374,9 +374,6 @@
     <t>PinPoint</t>
   </si>
   <si>
-    <t>Incertitude</t>
-  </si>
-  <si>
     <t>Incertitude absolue</t>
   </si>
   <si>
@@ -403,16 +400,53 @@
   <si>
     <t>Incertitudes</t>
   </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>élargie k=2 (%)</t>
+  </si>
+  <si>
+    <t>kQQ0 (%)</t>
+  </si>
+  <si>
+    <t>Ndeau (%)</t>
+  </si>
+  <si>
+    <t>Pinpoint</t>
+  </si>
+  <si>
+    <t>Incertitude (%)</t>
+  </si>
+  <si>
+    <t>Incertitude k=2 (%)</t>
+  </si>
+  <si>
+    <t>Incertitude absolue (Gy)</t>
+  </si>
+  <si>
+    <t>ER ref 1 (%)</t>
+  </si>
+  <si>
+    <t>Ecart (mGy)</t>
+  </si>
+  <si>
+    <t/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -841,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -897,9 +931,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -953,9 +984,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1165,18 +1193,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1201,9 +1217,6 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1249,9 +1262,103 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1280,12 +1387,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1321,43 +1443,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4298,8 +4393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2AC7B24-2B93-C343-AFA4-0AA761761623}">
   <dimension ref="B1:R37"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="97" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4309,30 +4404,30 @@
   <sheetData>
     <row r="1" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="6">
         <v>21</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>22</v>
       </c>
       <c r="F2" s="2">
         <v>1013.25</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="8">
         <v>1015</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="5">
@@ -4353,243 +4448,243 @@
       <c r="C5" s="15"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="143" t="s">
+      <c r="B6" s="168" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="143"/>
-      <c r="I6" s="143"/>
-      <c r="J6" s="143"/>
+      <c r="C6" s="168"/>
+      <c r="D6" s="168"/>
+      <c r="E6" s="168"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="168"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="168"/>
     </row>
     <row r="7" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-      <c r="C8" s="147" t="s">
+      <c r="C8" s="172" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="148"/>
-      <c r="E8" s="148"/>
-      <c r="F8" s="149"/>
-      <c r="G8" s="144" t="s">
+      <c r="D8" s="173"/>
+      <c r="E8" s="173"/>
+      <c r="F8" s="174"/>
+      <c r="G8" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="145"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="146"/>
+      <c r="H8" s="170"/>
+      <c r="I8" s="170"/>
+      <c r="J8" s="171"/>
     </row>
     <row r="9" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="30">
         <v>400</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <v>100</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="31">
         <v>-400</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <v>-100</v>
       </c>
-      <c r="G9" s="59">
+      <c r="G9" s="57">
         <v>400</v>
       </c>
-      <c r="H9" s="60">
+      <c r="H9" s="58">
         <v>100</v>
       </c>
-      <c r="I9" s="60">
+      <c r="I9" s="58">
         <v>-400</v>
       </c>
-      <c r="J9" s="61">
+      <c r="J9" s="59">
         <v>-100</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="56" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="11">
         <v>29.69</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="54">
         <v>29.5</v>
       </c>
-      <c r="E10" s="56">
+      <c r="E10" s="54">
         <v>29.8</v>
       </c>
-      <c r="F10" s="64">
+      <c r="F10" s="62">
         <v>29.61</v>
       </c>
-      <c r="G10" s="49">
+      <c r="G10" s="47">
         <v>36.64</v>
       </c>
-      <c r="H10" s="55">
+      <c r="H10" s="53">
         <v>36.15</v>
       </c>
-      <c r="I10" s="55">
+      <c r="I10" s="53">
         <v>36.78</v>
       </c>
-      <c r="J10" s="65">
+      <c r="J10" s="63">
         <v>36.28</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="56" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="11">
         <v>29.7</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="54">
         <v>29.52</v>
       </c>
-      <c r="E11" s="56">
+      <c r="E11" s="54">
         <v>29.82</v>
       </c>
-      <c r="F11" s="64">
+      <c r="F11" s="62">
         <v>29.59</v>
       </c>
       <c r="G11" s="1">
         <v>36.619999999999997</v>
       </c>
-      <c r="H11" s="56">
+      <c r="H11" s="54">
         <v>36.1</v>
       </c>
-      <c r="I11" s="56">
+      <c r="I11" s="54">
         <v>36.75</v>
       </c>
-      <c r="J11" s="64">
+      <c r="J11" s="62">
         <v>36.25</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="56" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="11">
         <v>29.73</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="54">
         <v>29.55</v>
       </c>
-      <c r="E12" s="56">
+      <c r="E12" s="54">
         <v>29.8</v>
       </c>
-      <c r="F12" s="64">
+      <c r="F12" s="62">
         <v>29.61</v>
       </c>
       <c r="G12" s="1">
         <v>36.61</v>
       </c>
-      <c r="H12" s="56">
+      <c r="H12" s="54">
         <v>36.08</v>
       </c>
-      <c r="I12" s="56">
+      <c r="I12" s="54">
         <v>36.729999999999997</v>
       </c>
-      <c r="J12" s="64">
+      <c r="J12" s="62">
         <v>36.21</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="52">
+      <c r="C13" s="50">
         <f>AVERAGE(C10:C12)</f>
         <v>29.706666666666667</v>
       </c>
-      <c r="D13" s="54">
+      <c r="D13" s="52">
         <f t="shared" ref="D13:E13" si="0">AVERAGE(D10:D12)</f>
         <v>29.52333333333333</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="52">
         <f t="shared" si="0"/>
         <v>29.806666666666668</v>
       </c>
-      <c r="F13" s="63">
+      <c r="F13" s="61">
         <f>AVERAGE(F10:F12)</f>
         <v>29.603333333333335</v>
       </c>
-      <c r="G13" s="54">
+      <c r="G13" s="52">
         <f>AVERAGE(G10:G12)</f>
         <v>36.623333333333328</v>
       </c>
-      <c r="H13" s="54">
+      <c r="H13" s="52">
         <f t="shared" ref="H13:J13" si="1">AVERAGE(H10:H12)</f>
         <v>36.11</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I13" s="52">
         <f t="shared" si="1"/>
         <v>36.75333333333333</v>
       </c>
-      <c r="J13" s="63">
+      <c r="J13" s="61">
         <f t="shared" si="1"/>
         <v>36.24666666666667</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="169">
+      <c r="C14" s="155">
         <f>P20+Q20*C13/D13+R20*(C13/D13)^2</f>
         <v>1.0019940684631883</v>
       </c>
-      <c r="D14" s="170"/>
-      <c r="E14" s="170"/>
-      <c r="F14" s="171"/>
-      <c r="G14" s="169">
+      <c r="D14" s="136"/>
+      <c r="E14" s="136"/>
+      <c r="F14" s="137"/>
+      <c r="G14" s="135">
         <f>P20+Q20*G13/H13+R20*(G13/H13)^2</f>
         <v>1.0046037597782551</v>
       </c>
-      <c r="H14" s="170"/>
-      <c r="I14" s="170"/>
-      <c r="J14" s="171"/>
+      <c r="H14" s="136"/>
+      <c r="I14" s="136"/>
+      <c r="J14" s="137"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="169">
+      <c r="C15" s="135">
         <f>(ABS(C13)+ABS(E13))/(2*ABS(C11))</f>
         <v>1.0019079685746353</v>
       </c>
-      <c r="D15" s="170"/>
-      <c r="E15" s="170"/>
-      <c r="F15" s="171"/>
-      <c r="G15" s="169">
+      <c r="D15" s="136"/>
+      <c r="E15" s="136"/>
+      <c r="F15" s="137"/>
+      <c r="G15" s="135">
         <f>(ABS(G13)+ABS(I13))/(2*ABS(G11))</f>
         <v>1.0018660112870927</v>
       </c>
-      <c r="H15" s="170"/>
-      <c r="I15" s="170"/>
-      <c r="J15" s="171"/>
+      <c r="H15" s="136"/>
+      <c r="I15" s="136"/>
+      <c r="J15" s="137"/>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="172">
+      <c r="C16" s="138">
         <f>(ABS(D13)+ABS(F13))/(2*ABS(D13))</f>
         <v>1.0013548605622673</v>
       </c>
-      <c r="D16" s="173"/>
-      <c r="E16" s="173"/>
-      <c r="F16" s="174"/>
-      <c r="G16" s="172">
+      <c r="D16" s="139"/>
+      <c r="E16" s="139"/>
+      <c r="F16" s="140"/>
+      <c r="G16" s="138">
         <f>(ABS(H13)+ABS(J13))/(2*ABS(H13))</f>
         <v>1.0018923659189514</v>
       </c>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="174"/>
+      <c r="H16" s="139"/>
+      <c r="I16" s="139"/>
+      <c r="J16" s="140"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
@@ -4601,47 +4696,47 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="143" t="s">
+      <c r="B18" s="168" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="143"/>
-      <c r="D18" s="143"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="143"/>
-      <c r="I18" s="143"/>
-      <c r="J18" s="143"/>
+      <c r="C18" s="168"/>
+      <c r="D18" s="168"/>
+      <c r="E18" s="168"/>
+      <c r="F18" s="168"/>
+      <c r="G18" s="168"/>
+      <c r="H18" s="168"/>
+      <c r="I18" s="168"/>
+      <c r="J18" s="168"/>
     </row>
     <row r="19" spans="2:18" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="O19" s="27" t="s">
+      <c r="O19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="P19" s="22" t="s">
+      <c r="P19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="Q19" s="28" t="s">
+      <c r="Q19" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="R19" s="29" t="s">
+      <c r="R19" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="147" t="s">
+      <c r="C20" s="172" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="148"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="149"/>
-      <c r="G20" s="144" t="s">
+      <c r="D20" s="173"/>
+      <c r="E20" s="173"/>
+      <c r="F20" s="174"/>
+      <c r="G20" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="145"/>
-      <c r="I20" s="145"/>
-      <c r="J20" s="146"/>
-      <c r="O20" s="26">
+      <c r="H20" s="170"/>
+      <c r="I20" s="170"/>
+      <c r="J20" s="171"/>
+      <c r="O20" s="25">
         <f>C9/D9</f>
         <v>4</v>
       </c>
@@ -4656,218 +4751,218 @@
       </c>
     </row>
     <row r="21" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="59">
+      <c r="C21" s="57">
         <v>400</v>
       </c>
-      <c r="D21" s="60">
+      <c r="D21" s="58">
         <v>100</v>
       </c>
-      <c r="E21" s="60">
+      <c r="E21" s="58">
         <v>-400</v>
       </c>
-      <c r="F21" s="61">
+      <c r="F21" s="59">
         <v>-100</v>
       </c>
-      <c r="G21" s="59">
+      <c r="G21" s="57">
         <v>400</v>
       </c>
-      <c r="H21" s="60">
+      <c r="H21" s="58">
         <v>100</v>
       </c>
-      <c r="I21" s="60">
+      <c r="I21" s="58">
         <v>-400</v>
       </c>
-      <c r="J21" s="61">
+      <c r="J21" s="59">
         <v>-100</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="48">
+      <c r="C22" s="46">
         <v>0.67420000000000002</v>
       </c>
-      <c r="D22" s="78">
+      <c r="D22" s="76">
         <v>0.66890000000000005</v>
       </c>
-      <c r="E22" s="78">
+      <c r="E22" s="76">
         <v>0.68500000000000005</v>
       </c>
-      <c r="F22" s="79">
+      <c r="F22" s="77">
         <v>0.68310000000000004</v>
       </c>
-      <c r="G22" s="49">
+      <c r="G22" s="47">
         <v>0.83120000000000005</v>
       </c>
-      <c r="H22" s="78">
+      <c r="H22" s="76">
         <v>0.8236</v>
       </c>
-      <c r="I22" s="78">
+      <c r="I22" s="76">
         <v>0.84789999999999999</v>
       </c>
-      <c r="J22" s="79">
+      <c r="J22" s="77">
         <v>0.84289999999999998</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="56" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="11">
         <v>0.67449999999999999</v>
       </c>
-      <c r="D23" s="77">
+      <c r="D23" s="75">
         <v>0.66959999999999997</v>
       </c>
-      <c r="E23" s="77">
+      <c r="E23" s="75">
         <v>0.68489999999999995</v>
       </c>
-      <c r="F23" s="76">
+      <c r="F23" s="74">
         <v>0.68340000000000001</v>
       </c>
       <c r="G23" s="1">
         <v>0.83130000000000004</v>
       </c>
-      <c r="H23" s="77">
+      <c r="H23" s="75">
         <v>0.82269999999999999</v>
       </c>
-      <c r="I23" s="77">
+      <c r="I23" s="75">
         <v>0.84699999999999998</v>
       </c>
-      <c r="J23" s="76">
+      <c r="J23" s="74">
         <v>0.84279999999999999</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="56" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="11">
         <v>0.67430000000000001</v>
       </c>
-      <c r="D24" s="77">
+      <c r="D24" s="75">
         <v>0.6694</v>
       </c>
-      <c r="E24" s="77">
+      <c r="E24" s="75">
         <v>0.68469999999999998</v>
       </c>
-      <c r="F24" s="76">
+      <c r="F24" s="74">
         <v>0.68340000000000001</v>
       </c>
       <c r="G24" s="1">
         <v>0.83089999999999997</v>
       </c>
-      <c r="H24" s="77">
+      <c r="H24" s="75">
         <v>0.82199999999999995</v>
       </c>
-      <c r="I24" s="77">
+      <c r="I24" s="75">
         <v>0.84640000000000004</v>
       </c>
-      <c r="J24" s="76">
+      <c r="J24" s="74">
         <v>0.84309999999999996</v>
       </c>
     </row>
     <row r="25" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="80">
+      <c r="C25" s="78">
         <f>AVERAGE(C22:C24)</f>
         <v>0.67433333333333334</v>
       </c>
-      <c r="D25" s="81">
+      <c r="D25" s="79">
         <f t="shared" ref="D25:J25" si="2">AVERAGE(D22:D24)</f>
         <v>0.66930000000000012</v>
       </c>
-      <c r="E25" s="81">
+      <c r="E25" s="79">
         <f t="shared" si="2"/>
         <v>0.68486666666666662</v>
       </c>
-      <c r="F25" s="66">
+      <c r="F25" s="64">
         <f t="shared" si="2"/>
         <v>0.68330000000000002</v>
       </c>
-      <c r="G25" s="81">
+      <c r="G25" s="79">
         <f t="shared" si="2"/>
         <v>0.83113333333333339</v>
       </c>
-      <c r="H25" s="81">
+      <c r="H25" s="79">
         <f>AVERAGE(H22:H24)</f>
         <v>0.82276666666666676</v>
       </c>
-      <c r="I25" s="81">
+      <c r="I25" s="79">
         <f t="shared" si="2"/>
         <v>0.84710000000000008</v>
       </c>
-      <c r="J25" s="66">
+      <c r="J25" s="64">
         <f t="shared" si="2"/>
         <v>0.84293333333333331</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="123">
+      <c r="C26" s="141">
         <f>P20+Q20*C25/D25+R20*(C25/D25)^2</f>
         <v>1.0024182592510269</v>
       </c>
-      <c r="D26" s="124"/>
-      <c r="E26" s="124"/>
-      <c r="F26" s="125"/>
-      <c r="G26" s="123">
+      <c r="D26" s="117"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="118"/>
+      <c r="G26" s="142">
         <f>P20+Q20*G25/H25+R20*(G25/H25)^2</f>
         <v>1.0032791544759843</v>
       </c>
-      <c r="H26" s="124"/>
-      <c r="I26" s="124"/>
-      <c r="J26" s="125"/>
+      <c r="H26" s="117"/>
+      <c r="I26" s="117"/>
+      <c r="J26" s="118"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="123">
-        <f>(ABS(C25)+ABS(E25))/(2*ABS(C25))</f>
-        <v>1.0078101828966881</v>
-      </c>
-      <c r="D27" s="124"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="125"/>
-      <c r="G27" s="123">
+      <c r="C27" s="141">
+        <f>(ABS(C25)+ABS(E25))/(2*ABS(C22))</f>
+        <v>1.0080094927321268</v>
+      </c>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="142">
         <f>(ABS(G25)+ABS(I25))/(2*ABS(G23))</f>
         <v>1.0094029431813625</v>
       </c>
-      <c r="H27" s="124"/>
-      <c r="I27" s="124"/>
-      <c r="J27" s="125"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="117"/>
+      <c r="J27" s="118"/>
     </row>
     <row r="28" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="126">
+      <c r="C28" s="143">
         <f>(ABS(D25)+ABS(F25))/(2*ABS(D25))</f>
         <v>1.0104586881816824</v>
       </c>
-      <c r="D28" s="127"/>
-      <c r="E28" s="127"/>
-      <c r="F28" s="128"/>
-      <c r="G28" s="126">
+      <c r="D28" s="120"/>
+      <c r="E28" s="120"/>
+      <c r="F28" s="121"/>
+      <c r="G28" s="119">
         <f>(ABS(H25)+ABS(J25))/(2*ABS(H25))</f>
         <v>1.0122553984523761</v>
       </c>
-      <c r="H28" s="127"/>
-      <c r="I28" s="127"/>
-      <c r="J28" s="128"/>
+      <c r="H28" s="120"/>
+      <c r="I28" s="120"/>
+      <c r="J28" s="121"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B30" s="143" t="s">
-        <v>66</v>
+      <c r="B30" s="168" t="s">
+        <v>65</v>
       </c>
       <c r="C30" s="175"/>
       <c r="D30" s="175"/>
@@ -4884,96 +4979,96 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="141" t="s">
+      <c r="F32" s="166" t="s">
         <v>55</v>
       </c>
-      <c r="G32" s="142"/>
-      <c r="H32" s="139" t="s">
+      <c r="G32" s="167"/>
+      <c r="H32" s="164" t="s">
         <v>56</v>
       </c>
-      <c r="I32" s="140"/>
+      <c r="I32" s="165"/>
     </row>
     <row r="33" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="135" t="s">
+      <c r="F33" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="G33" s="103" t="s">
+      <c r="G33" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="H33" s="135" t="s">
+      <c r="H33" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="I33" s="103" t="s">
+      <c r="I33" s="101" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="116" t="s">
+      <c r="B34" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="122">
+      <c r="C34" s="116">
         <f>0.2/C2/SQRT(12)</f>
         <v>2.7492869961410755E-3</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="116" t="s">
+      <c r="E34" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="136">
+      <c r="F34" s="129">
         <f>C14*SQRT((STDEV(C10:C12)/C13)^2+(STDEV(D10:D12)/D13)^2)</f>
         <v>1.1056709961229057E-3</v>
       </c>
-      <c r="G34" s="122">
+      <c r="G34" s="116">
         <f>G14*SQRT((STDEV(G10:G12)/G13)^2+(STDEV(H10:H12)/H13)^2)</f>
         <v>1.087085759540086E-3</v>
       </c>
-      <c r="H34" s="138">
+      <c r="H34" s="131">
         <f>C26*SQRT((STDEV(C22:C24)/C25)^2+(STDEV(D22:D24)/D25)^2)</f>
         <v>5.8580681886589005E-4</v>
       </c>
-      <c r="I34" s="133">
+      <c r="I34" s="126">
         <f>G26*SQRT((STDEV(G22:G24)/G25)^2+(STDEV(H22:H24)/H25)^2)</f>
         <v>1.0098186893410365E-3</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="134" t="s">
+      <c r="B35" s="127" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="133">
+      <c r="C35" s="126">
         <f>0.5/C3/SQRT(12)</f>
         <v>1.4220449980040044E-4</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="119" t="s">
+      <c r="E35" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="137">
+      <c r="F35" s="130">
         <f>C15*SQRT((STDEV(C10:C12)/C13)^2+(STDEV(E10:E12)/E13)^2)</f>
         <v>8.0222319277584934E-4</v>
       </c>
-      <c r="G35" s="115">
+      <c r="G35" s="109">
         <f>G15*SQRT((STDEV(G10:G12)/G13)^2+(STDEV(I10:I12)/I13)^2)</f>
         <v>8.0325666882393061E-4</v>
       </c>
-      <c r="H35" s="137">
+      <c r="H35" s="130">
         <f>C27*SQRT((STDEV(C22:C24)/C25)^2+(STDEV(E22:E24)/E25)^2)</f>
-        <v>3.2038183653242998E-4</v>
-      </c>
-      <c r="I35" s="115">
+        <v>3.2044519692727466E-4</v>
+      </c>
+      <c r="I35" s="109">
         <f>G27*SQRT((STDEV(G22:G24)/G25)^2+(STDEV(I22:I24)/I25)^2)</f>
         <v>9.3448530367910333E-4</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="119" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="115">
+      <c r="B36" s="113" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="109">
         <f>SQRT(C34^2+C35^2)</f>
         <v>2.7529622421882034E-3</v>
       </c>
@@ -5014,10 +5109,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A526C85-0CF3-CE40-BDDE-2C4E038089DC}">
-  <dimension ref="B3:S77"/>
+  <dimension ref="B3:S84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5025,72 +5120,74 @@
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.83203125" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H3" s="153" t="s">
+      <c r="H3" s="183" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="153"/>
+      <c r="I3" s="183"/>
     </row>
     <row r="4" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="147" t="s">
+      <c r="C4" s="172" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="149"/>
-      <c r="E4" s="145" t="s">
+      <c r="D4" s="174"/>
+      <c r="E4" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="146"/>
-      <c r="H4" s="154" t="s">
+      <c r="F4" s="171"/>
+      <c r="H4" s="184" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="155"/>
-      <c r="J4" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="L4" s="154" t="s">
+      <c r="I4" s="185"/>
+      <c r="J4" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" s="184" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="155"/>
-      <c r="N4" s="45" t="s">
-        <v>57</v>
+      <c r="M4" s="185"/>
+      <c r="N4" s="43" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="156" t="s">
+      <c r="B5" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="36">
-        <v>5.3560000000000003E-2</v>
+      <c r="I5" s="35">
+        <v>5.3650000000000003E-2</v>
       </c>
       <c r="J5" s="8">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L5" s="35" t="s">
+      <c r="L5" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="35">
+      <c r="M5" s="34">
         <v>2.3439999999999999</v>
       </c>
       <c r="N5" s="8">
@@ -5098,106 +5195,106 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B6" s="157"/>
-      <c r="C6" s="48">
+      <c r="B6" s="187"/>
+      <c r="C6" s="46">
         <v>29.7</v>
       </c>
-      <c r="D6" s="50">
+      <c r="D6" s="48">
         <v>19.7</v>
       </c>
       <c r="E6" s="1">
         <v>36.58</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="45">
         <v>28.6</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="157"/>
+      <c r="B7" s="187"/>
       <c r="C7" s="11">
         <v>29.66</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="45">
         <v>19.670000000000002</v>
       </c>
       <c r="E7" s="1">
         <v>36.57</v>
       </c>
-      <c r="F7" s="47">
+      <c r="F7" s="45">
         <v>28.54</v>
       </c>
-      <c r="H7" s="153" t="s">
+      <c r="H7" s="183" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="153"/>
+      <c r="I7" s="183"/>
     </row>
     <row r="8" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="157"/>
+      <c r="B8" s="187"/>
       <c r="C8" s="11">
         <v>29.66</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="45">
         <v>19.66</v>
       </c>
       <c r="E8" s="1">
         <v>36.58</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="45">
         <v>28.51</v>
       </c>
-      <c r="H8" s="154" t="s">
+      <c r="H8" s="184" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="155"/>
+      <c r="I8" s="185"/>
     </row>
     <row r="9" spans="2:14" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="157"/>
+      <c r="B9" s="187"/>
       <c r="C9" s="11">
         <v>29.69</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="62">
         <v>19.7</v>
       </c>
       <c r="E9" s="1">
         <v>36.57</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F9" s="45">
         <v>28.52</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="36">
+      <c r="I9" s="35">
         <v>5.398E-2</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="157"/>
+      <c r="B10" s="187"/>
       <c r="C10" s="11">
         <v>29.66</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="45">
         <v>19.66</v>
       </c>
       <c r="E10" s="1">
         <v>36.58</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="45">
         <v>28.52</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="157"/>
+      <c r="B11" s="187"/>
       <c r="C11" s="11">
         <v>29.63</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="45">
         <v>19.649999999999999</v>
       </c>
       <c r="E11" s="1">
         <v>36.619999999999997</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F11" s="45">
         <v>28.53</v>
       </c>
       <c r="H11" s="7"/>
@@ -5206,110 +5303,110 @@
       <c r="K11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="L11" s="38" t="s">
+      <c r="L11" s="37" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="157"/>
+      <c r="B12" s="187"/>
       <c r="C12" s="11">
         <v>29.63</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="45">
         <v>19.66</v>
       </c>
       <c r="E12" s="1">
         <v>36.58</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="45">
         <v>28.53</v>
       </c>
-      <c r="H12" s="159" t="s">
+      <c r="H12" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="160"/>
-      <c r="J12" s="161"/>
-      <c r="K12" s="102">
+      <c r="I12" s="190"/>
+      <c r="J12" s="191"/>
+      <c r="K12" s="100">
         <f>'Facteurs correctifs'!C4*'Facteurs correctifs'!C14*'Facteurs correctifs'!C15</f>
         <v>1.0055936117462898</v>
       </c>
-      <c r="L12" s="101">
+      <c r="L12" s="99">
         <f>'Facteurs correctifs'!C4*'Facteurs correctifs'!G14*'Facteurs correctifs'!G15</f>
         <v>1.0081704567515035</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="157"/>
+      <c r="B13" s="187"/>
       <c r="C13" s="11">
         <v>29.63</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="45">
         <v>19.68</v>
       </c>
       <c r="E13" s="1">
         <v>36.6</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F13" s="45">
         <v>28.53</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="157"/>
+      <c r="B14" s="187"/>
       <c r="C14" s="11">
         <v>29.64</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="45">
         <v>19.649999999999999</v>
       </c>
       <c r="E14" s="1">
         <v>36.58</v>
       </c>
-      <c r="F14" s="47">
+      <c r="F14" s="45">
         <v>28.54</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="158"/>
+      <c r="B15" s="188"/>
       <c r="C15" s="12">
         <v>29.69</v>
       </c>
-      <c r="D15" s="75">
+      <c r="D15" s="73">
         <v>19.66</v>
       </c>
       <c r="E15" s="1">
         <v>36.590000000000003</v>
       </c>
-      <c r="F15" s="47">
+      <c r="F15" s="45">
         <v>28.53</v>
       </c>
-      <c r="H15" s="45" t="s">
+      <c r="H15" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="52">
+      <c r="C16" s="50">
         <f>AVERAGE(C5:C15)</f>
         <v>29.658999999999999</v>
       </c>
-      <c r="D16" s="53">
+      <c r="D16" s="51">
         <f>AVERAGE(D6:D15)</f>
         <v>19.669</v>
       </c>
-      <c r="E16" s="54">
+      <c r="E16" s="52">
         <f>AVERAGE(E5:E15)</f>
         <v>36.585000000000001</v>
       </c>
-      <c r="F16" s="53">
+      <c r="F16" s="51">
         <f>AVERAGE(F6:F15)</f>
         <v>28.535000000000004</v>
       </c>
-      <c r="H16" s="130">
+      <c r="H16" s="123">
         <v>0.5</v>
       </c>
       <c r="I16" s="3">
@@ -5317,7 +5414,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H17" s="130">
+      <c r="H17" s="123">
         <v>0.53</v>
       </c>
       <c r="I17" s="3">
@@ -5332,8 +5429,8 @@
       <c r="D18" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="H18" s="130">
+      <c r="E18" s="19"/>
+      <c r="H18" s="123">
         <v>0.56000000000000005</v>
       </c>
       <c r="I18" s="3">
@@ -5341,7 +5438,7 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="40" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="6">
@@ -5350,8 +5447,8 @@
       <c r="D19" s="2">
         <v>0.78100000000000003</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="H19" s="130">
+      <c r="E19" s="20"/>
+      <c r="H19" s="123">
         <v>0.59</v>
       </c>
       <c r="I19" s="3">
@@ -5359,19 +5456,19 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="67">
+      <c r="C20" s="65">
         <f>D16/C16</f>
         <v>0.66317138136821885</v>
       </c>
-      <c r="D20" s="68">
+      <c r="D20" s="66">
         <f>F16/E16</f>
         <v>0.77996446631132987</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="H20" s="130">
+      <c r="E20" s="20"/>
+      <c r="H20" s="123">
         <v>0.62</v>
       </c>
       <c r="I20" s="3">
@@ -5379,19 +5476,19 @@
       </c>
     </row>
     <row r="21" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="69">
+      <c r="C21" s="67">
         <f>ABS(C19-C20)/C19*100</f>
         <v>0.12479196261764851</v>
       </c>
-      <c r="D21" s="70">
+      <c r="D21" s="68">
         <f>ABS(D19-D20)/D19*100</f>
         <v>0.13259074118695952</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="H21" s="130">
+      <c r="E21" s="20"/>
+      <c r="H21" s="123">
         <v>0.65</v>
       </c>
       <c r="I21" s="3">
@@ -5402,15 +5499,15 @@
       <c r="B22" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="73">
+      <c r="C22" s="71">
         <f>(I19-I18)/(H19-H18)*C20+I18-(I19-I18)/(H19-H18)*H18</f>
         <v>0.9965609539543927</v>
       </c>
-      <c r="D22" s="74">
+      <c r="D22" s="72">
         <f>(I22-I21)/(H22-H21)*D20+I21-(I22-I21)/(H22-H21)*H21</f>
         <v>0.97667140449182266</v>
       </c>
-      <c r="H22" s="130">
+      <c r="H22" s="123">
         <v>0.68</v>
       </c>
       <c r="I22" s="3">
@@ -5418,7 +5515,7 @@
       </c>
     </row>
     <row r="23" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H23" s="130">
+      <c r="H23" s="123">
         <v>0.7</v>
       </c>
       <c r="I23" s="3">
@@ -5426,17 +5523,17 @@
       </c>
     </row>
     <row r="24" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="162" t="s">
+      <c r="B24" s="192" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="163"/>
+      <c r="C24" s="194"/>
       <c r="D24" s="14" t="s">
         <v>0</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="130">
+      <c r="H24" s="123">
         <v>0.72</v>
       </c>
       <c r="I24" s="3">
@@ -5444,19 +5541,19 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="150" t="s">
+      <c r="B25" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="117">
+      <c r="D25" s="111">
         <v>1.589</v>
       </c>
-      <c r="E25" s="118">
+      <c r="E25" s="112">
         <v>1.907</v>
       </c>
-      <c r="H25" s="130">
+      <c r="H25" s="123">
         <v>0.74</v>
       </c>
       <c r="I25" s="3">
@@ -5464,19 +5561,19 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="151"/>
-      <c r="C26" s="44" t="s">
+      <c r="B26" s="181"/>
+      <c r="C26" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="69">
+      <c r="D26" s="67">
         <f>C16*I5*K12*C22</f>
-        <v>1.5919280870933372</v>
-      </c>
-      <c r="E26" s="70">
+        <v>1.5946030969484231</v>
+      </c>
+      <c r="E26" s="68">
         <f>E16*I5*L12*D22</f>
-        <v>1.9294168496395252</v>
-      </c>
-      <c r="H26" s="130">
+        <v>1.9326589615974705</v>
+      </c>
+      <c r="H26" s="123">
         <v>0.76</v>
       </c>
       <c r="I26" s="3">
@@ -5484,19 +5581,19 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="152"/>
-      <c r="C27" s="45" t="s">
+      <c r="B27" s="182"/>
+      <c r="C27" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="72">
+      <c r="D27" s="70">
         <f>ABS(D25-D26)/D25*100</f>
-        <v>0.18427231550265893</v>
-      </c>
-      <c r="E27" s="63">
+        <v>0.35261780669748849</v>
+      </c>
+      <c r="E27" s="61">
         <f>ABS(E25-E26)/E25*100</f>
-        <v>1.1755033895923006</v>
-      </c>
-      <c r="H27" s="130">
+        <v>1.3455145043246197</v>
+      </c>
+      <c r="H27" s="123">
         <v>0.78</v>
       </c>
       <c r="I27" s="3">
@@ -5504,7 +5601,7 @@
       </c>
     </row>
     <row r="28" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H28" s="130">
+      <c r="H28" s="123">
         <v>0.8</v>
       </c>
       <c r="I28" s="3">
@@ -5515,10 +5612,10 @@
       <c r="C29" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="120" t="s">
+      <c r="D29" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="H29" s="130">
+      <c r="H29" s="123">
         <v>0.82</v>
       </c>
       <c r="I29" s="3">
@@ -5526,16 +5623,16 @@
       </c>
     </row>
     <row r="30" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="117">
+      <c r="B30" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="111">
         <f>D26*SQRT((STDEV(C6:C15)/C16)^2+(1/100)^2+'Facteurs correctifs'!C36^2+('Facteurs correctifs'!F34/'Facteurs correctifs'!C14)^2+('Facteurs correctifs'!F35/'Facteurs correctifs'!C15)^2+('Mesures Clinac 2'!J5/100)^2)</f>
-        <v>1.8870044756363485E-2</v>
-      </c>
-      <c r="D30" s="118">
+        <v>1.8901753196021304E-2</v>
+      </c>
+      <c r="D30" s="112">
         <f>E26*SQRT((STDEV(E6:E15)/E16)^2+(1/100)^2+'Facteurs correctifs'!C36^2+('Facteurs correctifs'!G34/'Facteurs correctifs'!G14)^2+('Facteurs correctifs'!G34/'Facteurs correctifs'!G15)^2+('Mesures Clinac 2'!J5/100)^2)</f>
-        <v>2.2857465704318375E-2</v>
+        <v>2.2895874440565362E-2</v>
       </c>
       <c r="H30" s="8">
         <v>0.84</v>
@@ -5545,870 +5642,1352 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="67">
+      <c r="B31" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="65">
         <f>2*C30</f>
-        <v>3.7740089512726969E-2</v>
-      </c>
-      <c r="D31" s="68">
+        <v>3.7803506392042607E-2</v>
+      </c>
+      <c r="D31" s="66">
         <f>2*D30</f>
-        <v>4.571493140863675E-2</v>
+        <v>4.5791748881130724E-2</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="57">
+      <c r="B32" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="55">
         <f>C31/D26*100</f>
-        <v>2.3707157263388496</v>
-      </c>
-      <c r="D32" s="62">
+        <v>2.3707157263388501</v>
+      </c>
+      <c r="D32" s="60">
         <f>D31/E26*100</f>
         <v>2.3693652005359915</v>
       </c>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B34" s="164" t="s">
+      <c r="B34" s="195" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="164"/>
-      <c r="D34" s="164"/>
-      <c r="E34" s="164"/>
-      <c r="F34" s="164"/>
-      <c r="G34" s="164"/>
-      <c r="H34" s="164"/>
-      <c r="I34" s="164"/>
-      <c r="J34" s="164"/>
-      <c r="K34" s="164"/>
-      <c r="L34" s="164"/>
+      <c r="C34" s="195"/>
+      <c r="D34" s="195"/>
+      <c r="E34" s="195"/>
+      <c r="F34" s="195"/>
+      <c r="G34" s="195"/>
+      <c r="H34" s="195"/>
+      <c r="I34" s="195"/>
+      <c r="J34" s="195"/>
+      <c r="K34" s="195"/>
+      <c r="L34" s="195"/>
     </row>
     <row r="35" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
-      <c r="C36" s="147" t="s">
+      <c r="C36" s="172" t="s">
         <v>0</v>
       </c>
-      <c r="D36" s="149"/>
-      <c r="E36" s="145" t="s">
+      <c r="D36" s="174"/>
+      <c r="E36" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="F36" s="146"/>
+      <c r="F36" s="171"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="147" t="s">
+      <c r="I36" s="172" t="s">
         <v>0</v>
       </c>
-      <c r="J36" s="149"/>
-      <c r="K36" s="145" t="s">
+      <c r="J36" s="174"/>
+      <c r="K36" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="L36" s="146"/>
-      <c r="P36" s="82"/>
-      <c r="Q36" s="82"/>
-      <c r="R36" s="82"/>
-      <c r="S36" s="82"/>
+      <c r="L36" s="171"/>
+      <c r="P36" s="80"/>
+      <c r="Q36" s="80"/>
+      <c r="R36" s="80"/>
+      <c r="S36" s="80"/>
     </row>
     <row r="37" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="156" t="s">
+      <c r="B37" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="23">
+      <c r="C37" s="22">
         <v>1</v>
       </c>
-      <c r="D37" s="46">
+      <c r="D37" s="44">
         <v>-1</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E37" s="22">
         <v>1</v>
       </c>
-      <c r="F37" s="46">
+      <c r="F37" s="44">
         <v>-1</v>
       </c>
-      <c r="H37" s="156" t="s">
+      <c r="H37" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="I37" s="23" t="s">
+      <c r="I37" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J37" s="46" t="s">
+      <c r="J37" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="K37" s="23" t="s">
+      <c r="K37" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="L37" s="46" t="s">
+      <c r="L37" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="P37" s="82"/>
-      <c r="Q37" s="82"/>
-      <c r="R37" s="82"/>
-      <c r="S37" s="82"/>
-    </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B38" s="157"/>
+      <c r="O37" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="P37" s="6">
+        <v>21.4</v>
+      </c>
+      <c r="Q37" s="80"/>
+      <c r="R37" s="80"/>
+      <c r="S37" s="80"/>
+    </row>
+    <row r="38" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="187"/>
       <c r="C38" s="11">
         <v>29.76</v>
       </c>
-      <c r="D38" s="47">
+      <c r="D38" s="45">
         <v>29.75</v>
       </c>
       <c r="E38" s="1">
         <v>36.659999999999997</v>
       </c>
-      <c r="F38" s="47">
+      <c r="F38" s="45">
         <v>36.659999999999997</v>
       </c>
-      <c r="H38" s="157"/>
+      <c r="H38" s="187"/>
       <c r="I38" s="11">
         <v>29.53</v>
       </c>
-      <c r="J38" s="47">
+      <c r="J38" s="45">
         <v>29.88</v>
       </c>
       <c r="K38" s="1">
         <v>36.46</v>
       </c>
-      <c r="L38" s="47">
+      <c r="L38" s="45">
         <v>36.76</v>
       </c>
-      <c r="P38" s="82"/>
-      <c r="Q38" s="82"/>
-      <c r="R38" s="82"/>
-      <c r="S38" s="82"/>
-    </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B39" s="157"/>
+      <c r="O38" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="P38" s="8">
+        <v>1017</v>
+      </c>
+      <c r="Q38" s="80"/>
+      <c r="R38" s="80"/>
+      <c r="S38" s="80"/>
+    </row>
+    <row r="39" spans="2:19" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="187"/>
       <c r="C39" s="11">
         <v>29.76</v>
       </c>
-      <c r="D39" s="47">
+      <c r="D39" s="45">
         <v>29.79</v>
       </c>
       <c r="E39" s="1">
         <v>36.659999999999997</v>
       </c>
-      <c r="F39" s="47">
+      <c r="F39" s="45">
         <v>36.659999999999997</v>
       </c>
-      <c r="H39" s="157"/>
+      <c r="H39" s="187"/>
       <c r="I39" s="11">
         <v>29.55</v>
       </c>
-      <c r="J39" s="47">
+      <c r="J39" s="45">
         <v>29.83</v>
       </c>
       <c r="K39" s="1">
         <v>36.450000000000003</v>
       </c>
-      <c r="L39" s="47">
+      <c r="L39" s="45">
         <v>36.75</v>
       </c>
-      <c r="P39" s="82"/>
-      <c r="Q39" s="82"/>
-      <c r="R39" s="82"/>
-      <c r="S39" s="82"/>
-    </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B40" s="157"/>
+      <c r="O39" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="P39" s="17">
+        <f>('Facteurs correctifs'!F2*('Mesures Clinac 2'!P37+273.15))/(('Facteurs correctifs'!F3+273.15)*P38)</f>
+        <v>1.0010707869007027</v>
+      </c>
+      <c r="Q39" s="80"/>
+      <c r="R39" s="80"/>
+      <c r="S39" s="80"/>
+    </row>
+    <row r="40" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="187"/>
       <c r="C40" s="11">
         <v>29.8</v>
       </c>
-      <c r="D40" s="47">
+      <c r="D40" s="45">
         <v>29.75</v>
       </c>
       <c r="E40" s="1">
         <v>36.68</v>
       </c>
-      <c r="F40" s="47">
+      <c r="F40" s="45">
         <v>36.61</v>
       </c>
-      <c r="H40" s="157"/>
+      <c r="H40" s="187"/>
       <c r="I40" s="11">
         <v>29.56</v>
       </c>
-      <c r="J40" s="47">
+      <c r="J40" s="45">
         <v>29.88</v>
       </c>
       <c r="K40" s="1">
         <v>36.46</v>
       </c>
-      <c r="L40" s="47">
+      <c r="L40" s="45">
         <v>36.76</v>
       </c>
-      <c r="P40" s="82"/>
-      <c r="Q40" s="82"/>
-      <c r="R40" s="82"/>
-      <c r="S40" s="82"/>
-    </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B41" s="157"/>
+      <c r="O40" s="154" t="s">
+        <v>72</v>
+      </c>
+      <c r="P40" s="158">
+        <f>SQRT((0.2/P37/SQRT(12))^2+(0.5/P38/SQRT(12))^2)*100</f>
+        <v>0.27016289031902291</v>
+      </c>
+      <c r="Q40" s="80"/>
+      <c r="R40" s="80"/>
+      <c r="S40" s="80"/>
+    </row>
+    <row r="41" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="187"/>
       <c r="C41" s="11">
         <v>29.78</v>
       </c>
-      <c r="D41" s="47">
+      <c r="D41" s="45">
         <v>29.8</v>
       </c>
       <c r="E41" s="1">
         <v>36.69</v>
       </c>
-      <c r="F41" s="47">
+      <c r="F41" s="45">
         <v>36.630000000000003</v>
       </c>
-      <c r="H41" s="157"/>
+      <c r="H41" s="187"/>
       <c r="I41" s="11">
         <v>29.57</v>
       </c>
-      <c r="J41" s="47">
+      <c r="J41" s="45">
         <v>29.89</v>
       </c>
       <c r="K41" s="1">
         <v>36.46</v>
       </c>
-      <c r="L41" s="47">
+      <c r="L41" s="45">
         <v>36.75</v>
       </c>
-      <c r="P41" s="82"/>
-      <c r="Q41" s="82"/>
-      <c r="R41" s="82"/>
-      <c r="S41" s="82"/>
-    </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B42" s="157"/>
+      <c r="P41" s="80"/>
+      <c r="Q41" s="80"/>
+      <c r="R41" s="80"/>
+      <c r="S41" s="80"/>
+    </row>
+    <row r="42" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="187"/>
       <c r="C42" s="11">
         <v>29.8</v>
       </c>
-      <c r="D42" s="47">
+      <c r="D42" s="45">
         <v>29.78</v>
       </c>
       <c r="E42" s="1">
         <v>36.69</v>
       </c>
-      <c r="F42" s="47">
+      <c r="F42" s="45">
         <v>36.65</v>
       </c>
-      <c r="H42" s="157"/>
+      <c r="H42" s="187"/>
       <c r="I42" s="11">
         <v>29.54</v>
       </c>
-      <c r="J42" s="47">
+      <c r="J42" s="45">
         <v>29.87</v>
       </c>
       <c r="K42" s="1">
         <v>36.47</v>
       </c>
-      <c r="L42" s="47">
+      <c r="L42" s="45">
         <v>36.75</v>
       </c>
-      <c r="P42" s="82"/>
-      <c r="Q42" s="82"/>
-      <c r="R42" s="82"/>
-      <c r="S42" s="82"/>
-    </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B43" s="157"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="R42" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="S42" s="80"/>
+    </row>
+    <row r="43" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="187"/>
       <c r="C43" s="11">
         <v>29.79</v>
       </c>
-      <c r="D43" s="47">
+      <c r="D43" s="45">
         <v>29.8</v>
       </c>
       <c r="E43" s="1">
         <v>36.700000000000003</v>
       </c>
-      <c r="F43" s="47">
+      <c r="F43" s="45">
         <v>36.65</v>
       </c>
-      <c r="H43" s="157"/>
+      <c r="H43" s="187"/>
       <c r="I43" s="11">
         <v>29.56</v>
       </c>
-      <c r="J43" s="47">
+      <c r="J43" s="45">
         <v>29.86</v>
       </c>
       <c r="K43" s="1">
         <v>36.479999999999997</v>
       </c>
-      <c r="L43" s="47">
+      <c r="L43" s="45">
         <v>36.76</v>
       </c>
-      <c r="P43" s="82"/>
-      <c r="Q43" s="82"/>
-      <c r="R43" s="82"/>
-      <c r="S43" s="82"/>
+      <c r="N43" s="189" t="s">
+        <v>14</v>
+      </c>
+      <c r="O43" s="190"/>
+      <c r="P43" s="191"/>
+      <c r="Q43" s="100">
+        <f>P39*'Facteurs correctifs'!C14*'Facteurs correctifs'!C15</f>
+        <v>1.0049808108825731</v>
+      </c>
+      <c r="R43" s="99">
+        <f>P39*'Facteurs correctifs'!G14*'Facteurs correctifs'!G15</f>
+        <v>1.0075560855786416</v>
+      </c>
+      <c r="S43" s="80"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B44" s="157"/>
+      <c r="B44" s="187"/>
       <c r="C44" s="11">
         <v>29.79</v>
       </c>
-      <c r="D44" s="47">
+      <c r="D44" s="45">
         <v>29.8</v>
       </c>
       <c r="E44" s="1">
         <v>36.700000000000003</v>
       </c>
-      <c r="F44" s="47">
+      <c r="F44" s="45">
         <v>36.659999999999997</v>
       </c>
-      <c r="H44" s="157"/>
+      <c r="H44" s="187"/>
       <c r="I44" s="11">
         <v>29.56</v>
       </c>
-      <c r="J44" s="47">
+      <c r="J44" s="45">
         <v>29.88</v>
       </c>
       <c r="K44" s="1">
         <v>36.47</v>
       </c>
-      <c r="L44" s="47">
+      <c r="L44" s="45">
         <v>36.76</v>
       </c>
-      <c r="P44" s="82"/>
-      <c r="Q44" s="82"/>
-      <c r="R44" s="82"/>
-      <c r="S44" s="82"/>
+      <c r="P44" s="80"/>
+      <c r="Q44" s="80"/>
+      <c r="R44" s="80"/>
+      <c r="S44" s="80"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B45" s="157"/>
+      <c r="B45" s="187"/>
       <c r="C45" s="11">
         <v>29.78</v>
       </c>
-      <c r="D45" s="47">
+      <c r="D45" s="45">
         <v>29.79</v>
       </c>
       <c r="E45" s="1">
         <v>36.71</v>
       </c>
-      <c r="F45" s="47">
+      <c r="F45" s="45">
         <v>36.659999999999997</v>
       </c>
-      <c r="H45" s="157"/>
+      <c r="H45" s="187"/>
       <c r="I45" s="11">
         <v>29.52</v>
       </c>
-      <c r="J45" s="47">
+      <c r="J45" s="45">
         <v>29.84</v>
       </c>
       <c r="K45" s="1">
         <v>36.479999999999997</v>
       </c>
-      <c r="L45" s="47">
+      <c r="L45" s="45">
         <v>36.75</v>
       </c>
-      <c r="P45" s="82"/>
-      <c r="Q45" s="82"/>
-      <c r="R45" s="82"/>
-      <c r="S45" s="82"/>
+      <c r="P45" s="80"/>
+      <c r="Q45" s="80"/>
+      <c r="R45" s="80"/>
+      <c r="S45" s="80"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B46" s="157"/>
+      <c r="B46" s="187"/>
       <c r="C46" s="11">
         <v>29.79</v>
       </c>
-      <c r="D46" s="47">
+      <c r="D46" s="45">
         <v>29.79</v>
       </c>
       <c r="E46" s="1">
         <v>36.71</v>
       </c>
-      <c r="F46" s="47">
+      <c r="F46" s="45">
         <v>36.67</v>
       </c>
-      <c r="H46" s="157"/>
+      <c r="H46" s="187"/>
       <c r="I46" s="11">
         <v>29.57</v>
       </c>
-      <c r="J46" s="47">
+      <c r="J46" s="45">
         <v>29.87</v>
       </c>
       <c r="K46" s="1">
         <v>36.479999999999997</v>
       </c>
-      <c r="L46" s="47">
+      <c r="L46" s="45">
         <v>36.76</v>
       </c>
-      <c r="P46" s="82"/>
-      <c r="Q46" s="82"/>
-      <c r="R46" s="82"/>
-      <c r="S46" s="82"/>
+      <c r="P46" s="80"/>
+      <c r="Q46" s="80"/>
+      <c r="R46" s="80"/>
+      <c r="S46" s="80"/>
     </row>
     <row r="47" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="158"/>
+      <c r="B47" s="188"/>
       <c r="C47" s="11">
         <v>29.8</v>
       </c>
-      <c r="D47" s="47">
+      <c r="D47" s="45">
         <v>29.78</v>
       </c>
       <c r="E47" s="1">
         <v>36.700000000000003</v>
       </c>
-      <c r="F47" s="47">
+      <c r="F47" s="45">
         <v>36.67</v>
       </c>
-      <c r="H47" s="158"/>
+      <c r="H47" s="188"/>
       <c r="I47" s="11">
         <v>29.57</v>
       </c>
-      <c r="J47" s="47">
+      <c r="J47" s="45">
         <v>29.88</v>
       </c>
       <c r="K47" s="1">
         <v>36.49</v>
       </c>
-      <c r="L47" s="47">
+      <c r="L47" s="45">
         <v>36.76</v>
       </c>
-      <c r="P47" s="82"/>
-      <c r="Q47" s="82"/>
-      <c r="R47" s="82"/>
-      <c r="S47" s="82"/>
-    </row>
-    <row r="48" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P47" s="80"/>
+      <c r="Q47" s="80"/>
+      <c r="R47" s="80"/>
+      <c r="S47" s="80"/>
+    </row>
+    <row r="48" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B48" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="48">
+      <c r="C48" s="46">
         <f>AVERAGE(C38:C47)</f>
         <v>29.785000000000004</v>
       </c>
-      <c r="D48" s="50">
+      <c r="D48" s="48">
         <f>AVERAGE(D38:D47)</f>
         <v>29.783000000000005</v>
       </c>
-      <c r="E48" s="49">
+      <c r="E48" s="47">
         <f>AVERAGE(E38:E47)</f>
         <v>36.689999999999991</v>
       </c>
-      <c r="F48" s="51">
+      <c r="F48" s="49">
         <f>AVERAGE(F38:F47)</f>
         <v>36.652000000000001</v>
       </c>
       <c r="H48" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="I48" s="48">
+      <c r="I48" s="144">
         <f>AVERAGE(I38:I47)</f>
         <v>29.553000000000004</v>
       </c>
-      <c r="J48" s="2">
+      <c r="J48" s="112">
         <f>AVERAGE(J38:J47)</f>
         <v>29.867999999999995</v>
       </c>
-      <c r="K48" s="49">
+      <c r="K48" s="145">
         <f>AVERAGE(K37:K47)</f>
         <v>36.470000000000006</v>
       </c>
-      <c r="L48" s="2">
+      <c r="L48" s="112">
         <f>AVERAGE(L38:L47)</f>
         <v>36.755999999999993</v>
       </c>
-      <c r="P48" s="82"/>
-      <c r="Q48" s="82"/>
-      <c r="R48" s="82"/>
-      <c r="S48" s="82"/>
+      <c r="P48" s="80"/>
+      <c r="Q48" s="80"/>
+      <c r="R48" s="80"/>
+      <c r="S48" s="80"/>
     </row>
     <row r="49" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="40" t="s">
+      <c r="B49" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="111">
+      <c r="C49" s="160">
         <f>STDEV(C38:C47)</f>
         <v>1.5092308563561843E-2</v>
       </c>
-      <c r="D49" s="112">
+      <c r="D49" s="162">
         <f>STDEV(D38:D47)</f>
         <v>1.8885620632287128E-2</v>
       </c>
-      <c r="E49" s="113">
+      <c r="E49" s="159">
         <f>STDEV(E38:E47)</f>
         <v>1.8257418583507525E-2</v>
       </c>
-      <c r="F49" s="114">
+      <c r="F49" s="163">
         <f t="shared" ref="F49" si="0">STDEV(F38:F47)</f>
         <v>1.8737959096739819E-2</v>
       </c>
-      <c r="H49" s="40" t="s">
+      <c r="H49" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="I49" s="111">
+      <c r="I49" s="160">
         <f>STDEV(I38:I47)</f>
         <v>1.7669811040931332E-2</v>
       </c>
-      <c r="J49" s="115">
+      <c r="J49" s="68">
         <f>STDEV(J38:J47)</f>
         <v>1.932183566158616E-2</v>
       </c>
-      <c r="K49" s="113">
+      <c r="K49" s="159">
         <f t="shared" ref="K49:L49" si="1">STDEV(K38:K47)</f>
         <v>1.2472191289245255E-2</v>
       </c>
-      <c r="L49" s="115">
+      <c r="L49" s="68">
         <f t="shared" si="1"/>
         <v>5.1639777949421956E-3</v>
       </c>
-      <c r="P49" s="82"/>
-      <c r="Q49" s="82"/>
-      <c r="R49" s="82"/>
-      <c r="S49" s="82"/>
+      <c r="P49" s="80"/>
+      <c r="Q49" s="80"/>
+      <c r="R49" s="80"/>
+      <c r="S49" s="80"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="P50" s="82"/>
-      <c r="Q50" s="82"/>
-      <c r="R50" s="82"/>
-      <c r="S50" s="82"/>
+      <c r="B50" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="144">
+        <f>C48*I5*C22*Q43</f>
+        <v>1.6004015647061089</v>
+      </c>
+      <c r="D50" s="112">
+        <f>D48*I5*C22*Q43</f>
+        <v>1.6002941011127094</v>
+      </c>
+      <c r="E50" s="145">
+        <f>E48*I5*D22*R43</f>
+        <v>1.9370246208965465</v>
+      </c>
+      <c r="F50" s="112">
+        <f>F48*I5*D22*R43</f>
+        <v>1.9350184356800282</v>
+      </c>
+      <c r="H50" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="I50" s="144">
+        <f>I48*I5*C22*Q43</f>
+        <v>1.5879357878717355</v>
+      </c>
+      <c r="J50" s="112">
+        <f>J48*I5*C22*Q43</f>
+        <v>1.604861303832199</v>
+      </c>
+      <c r="K50" s="145">
+        <f>K48*I5*D22*R43</f>
+        <v>1.9254098643798605</v>
+      </c>
+      <c r="L50" s="112">
+        <f>L48*D22*I5*R43</f>
+        <v>1.9405090478515528</v>
+      </c>
+      <c r="P50" s="80"/>
+      <c r="Q50" s="80"/>
+      <c r="R50" s="80"/>
+      <c r="S50" s="80"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B51" s="164" t="s">
+      <c r="B51" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="146">
+        <f>C50*SQRT((C49/C48)^2+(J5/100)^2+(P40/100)^2+('Facteurs correctifs'!F34/'Facteurs correctifs'!C14)^2+('Facteurs correctifs'!F35/'Facteurs correctifs'!C15)^2+(1/100)^2)</f>
+        <v>1.8913490760212533E-2</v>
+      </c>
+      <c r="D51" s="66">
+        <f>D50*SQRT((D49/D48)^2+(J5/100)^2+(P40/100)^2+('Facteurs correctifs'!F34/'Facteurs correctifs'!C14)^2+('Facteurs correctifs'!F35/'Facteurs correctifs'!C15)^2+(1/100)^2)</f>
+        <v>1.8922058509497686E-2</v>
+      </c>
+      <c r="E51" s="147">
+        <f>E50*SQRT((E49/E48)^2+(J5/100)^2+(P40/100)^2+('Facteurs correctifs'!H34/'Facteurs correctifs'!G14)^2+('Facteurs correctifs'!G35/'Facteurs correctifs'!G15)^2+(1/100)^2)</f>
+        <v>2.2819043626082221E-2</v>
+      </c>
+      <c r="F51" s="66">
+        <f>F50*SQRT((F49/F48)^2+(J5/100)^2+(P40/100)^2+('Facteurs correctifs'!G34/'Facteurs correctifs'!G14)^2+('Facteurs correctifs'!G35/'Facteurs correctifs'!G15)^2+(1/100)^2)</f>
+        <v>2.2864675498405193E-2</v>
+      </c>
+      <c r="H51" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="I51" s="146">
+        <f>I50*SQRT((I49/I48)^2+(J5/100)^2+(P40/100)^2+('Facteurs correctifs'!F34/'Facteurs correctifs'!C14)^2+('Facteurs correctifs'!F35/'Facteurs correctifs'!C15)^2+(1/100)^2)</f>
+        <v>1.8772937040934839E-2</v>
+      </c>
+      <c r="J51" s="66">
+        <f>J50*SQRT((J49/J48)^2+(J5/100)^2+(P40/100)^2+('Facteurs correctifs'!F34/'Facteurs correctifs'!C14)^2+('Facteurs correctifs'!F35/'Facteurs correctifs'!C15)^2+(1/100)^2)</f>
+        <v>1.8977174378685829E-2</v>
+      </c>
+      <c r="K51" s="147">
+        <f>K50*SQRT((K49/K48)^2+(J5/100)^2+(P40/100)^2+('Facteurs correctifs'!G34/'Facteurs correctifs'!G14)^2+('Facteurs correctifs'!H35/'Facteurs correctifs'!G15)^2+(1/100)^2)</f>
+        <v>2.2695266347445293E-2</v>
+      </c>
+      <c r="L51" s="66">
+        <f>L50*SQRT((L49/L48)^2+(J5/100)^2+(P40/100)^2+('Facteurs correctifs'!G34/'Facteurs correctifs'!G14)^2+('Facteurs correctifs'!G35/'Facteurs correctifs'!G15)^2+(1/100)^2)</f>
+        <v>2.2909704902733707E-2</v>
+      </c>
+      <c r="P51" s="80"/>
+      <c r="Q51" s="80"/>
+      <c r="R51" s="80"/>
+      <c r="S51" s="80"/>
+    </row>
+    <row r="52" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B52" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" s="146">
+        <f>C51/C50*100</f>
+        <v>1.1817965676436792</v>
+      </c>
+      <c r="D52" s="66">
+        <f t="shared" ref="D52:F52" si="2">D51/D50*100</f>
+        <v>1.182411314041643</v>
+      </c>
+      <c r="E52" s="147">
+        <f t="shared" si="2"/>
+        <v>1.1780461321921911</v>
+      </c>
+      <c r="F52" s="66">
+        <f t="shared" si="2"/>
+        <v>1.1816257187425609</v>
+      </c>
+      <c r="H52" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="I52" s="146">
+        <f>I51/I50*100</f>
+        <v>1.182222680811021</v>
+      </c>
+      <c r="J52" s="66">
+        <f t="shared" ref="J52:L52" si="3">J51/J50*100</f>
+        <v>1.1824806500954828</v>
+      </c>
+      <c r="K52" s="147">
+        <f t="shared" si="3"/>
+        <v>1.1787239053517069</v>
+      </c>
+      <c r="L52" s="66">
+        <f t="shared" si="3"/>
+        <v>1.1806028386262015</v>
+      </c>
+      <c r="P52" s="80"/>
+      <c r="R52" s="80"/>
+      <c r="S52" s="80"/>
+    </row>
+    <row r="53" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" s="160">
+        <f>C52*2</f>
+        <v>2.3635931352873585</v>
+      </c>
+      <c r="D53" s="68">
+        <f t="shared" ref="D53:F53" si="4">D52*2</f>
+        <v>2.364822628083286</v>
+      </c>
+      <c r="E53" s="159">
+        <f t="shared" si="4"/>
+        <v>2.3560922643843822</v>
+      </c>
+      <c r="F53" s="68">
+        <f t="shared" si="4"/>
+        <v>2.3632514374851219</v>
+      </c>
+      <c r="H53" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="I53" s="160">
+        <f>I52*2</f>
+        <v>2.364445361622042</v>
+      </c>
+      <c r="J53" s="68">
+        <f t="shared" ref="J53:L53" si="5">J52*2</f>
+        <v>2.3649613001909655</v>
+      </c>
+      <c r="K53" s="159">
+        <f t="shared" si="5"/>
+        <v>2.3574478107034138</v>
+      </c>
+      <c r="L53" s="68">
+        <f t="shared" si="5"/>
+        <v>2.361205677252403</v>
+      </c>
+      <c r="P53" s="80"/>
+      <c r="Q53" s="80"/>
+      <c r="R53" s="80"/>
+      <c r="S53" s="80"/>
+    </row>
+    <row r="54" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B54" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="144">
+        <f>ABS(C50-D26)*1000</f>
+        <v>5.7984677576858878</v>
+      </c>
+      <c r="D54" s="112">
+        <f>ABS(D50-D26)*1000</f>
+        <v>5.6910041642863618</v>
+      </c>
+      <c r="E54" s="144">
+        <f>ABS(E50-$E$26)*1000</f>
+        <v>4.3656592990759524</v>
+      </c>
+      <c r="F54" s="112">
+        <f>ABS(F50-$E$26)*1000</f>
+        <v>2.3594740825576554</v>
+      </c>
+      <c r="H54" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="I54" s="144">
+        <f>ABS(I50-D26)*1000</f>
+        <v>6.6673090766875553</v>
+      </c>
+      <c r="J54" s="112">
+        <f>ABS(J50-D26)*1000</f>
+        <v>10.258206883775989</v>
+      </c>
+      <c r="K54" s="145">
+        <f>ABS(K50-E26)*1000</f>
+        <v>7.2490972176100232</v>
+      </c>
+      <c r="L54" s="112">
+        <f>ABS(L50-E26)*1000</f>
+        <v>7.8500862540822336</v>
+      </c>
+      <c r="P54" s="80"/>
+      <c r="Q54" s="80"/>
+      <c r="R54" s="80"/>
+      <c r="S54" s="80"/>
+    </row>
+    <row r="55" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="160">
+        <f>C54/1000/D26*100</f>
+        <v>0.36363078491333434</v>
+      </c>
+      <c r="D55" s="68">
+        <f>D54/1000/D26*100</f>
+        <v>0.35689157854874248</v>
+      </c>
+      <c r="E55" s="159">
+        <f>E54/1000/E26*100</f>
+        <v>0.22588875667269542</v>
+      </c>
+      <c r="F55" s="68">
+        <f>F54/1000/E26*100</f>
+        <v>0.1220843474943657</v>
+      </c>
+      <c r="H55" s="104" t="s">
+        <v>13</v>
+      </c>
+      <c r="I55" s="160">
+        <f>I54/1000/D26*100</f>
+        <v>0.41811715338109667</v>
+      </c>
+      <c r="J55" s="68">
+        <f>J54/1000/D26*100</f>
+        <v>0.64330784904450655</v>
+      </c>
+      <c r="K55" s="159">
+        <f>K54/1000/E26*100</f>
+        <v>0.37508413857032308</v>
+      </c>
+      <c r="L55" s="68">
+        <f>L54/1000/E26*100</f>
+        <v>0.40618062524562626</v>
+      </c>
+      <c r="P55" s="80"/>
+      <c r="Q55" s="80"/>
+      <c r="R55" s="80"/>
+      <c r="S55" s="80"/>
+    </row>
+    <row r="56" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="P56" s="80"/>
+      <c r="Q56" s="80"/>
+      <c r="R56" s="80"/>
+      <c r="S56" s="80"/>
+    </row>
+    <row r="57" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B57" s="195" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="164"/>
-      <c r="D51" s="164"/>
-      <c r="E51" s="164"/>
-      <c r="F51" s="164"/>
-      <c r="G51" s="164"/>
-      <c r="H51" s="164"/>
-      <c r="I51" s="164"/>
-      <c r="J51" s="164"/>
-      <c r="K51" s="164"/>
-      <c r="L51" s="164"/>
-      <c r="P51" s="82"/>
-      <c r="Q51" s="82"/>
-      <c r="R51" s="82"/>
-      <c r="S51" s="82"/>
-    </row>
-    <row r="52" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="P52" s="82"/>
-      <c r="Q52" s="82"/>
-      <c r="R52" s="82"/>
-      <c r="S52" s="82"/>
-    </row>
-    <row r="53" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P53" s="82"/>
-      <c r="Q53" s="82"/>
-      <c r="R53" s="82"/>
-      <c r="S53" s="82"/>
-    </row>
-    <row r="54" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-      <c r="C54" s="14" t="s">
+      <c r="C57" s="195"/>
+      <c r="D57" s="195"/>
+      <c r="E57" s="195"/>
+      <c r="F57" s="195"/>
+      <c r="G57" s="195"/>
+      <c r="H57" s="195"/>
+      <c r="I57" s="195"/>
+      <c r="J57" s="195"/>
+      <c r="K57" s="195"/>
+      <c r="L57" s="195"/>
+      <c r="P57" s="80"/>
+      <c r="Q57" s="80"/>
+      <c r="R57" s="80"/>
+      <c r="S57" s="80"/>
+    </row>
+    <row r="58" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="P58" s="80"/>
+      <c r="Q58" s="80"/>
+      <c r="R58" s="80"/>
+      <c r="S58" s="80"/>
+    </row>
+    <row r="59" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P59" s="80"/>
+      <c r="Q59" s="80"/>
+      <c r="R59" s="80"/>
+      <c r="S59" s="80"/>
+    </row>
+    <row r="60" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+      <c r="C60" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="D60" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F54" s="100"/>
-      <c r="P54" s="82"/>
-      <c r="Q54" s="82"/>
-      <c r="R54" s="82"/>
-      <c r="S54" s="82"/>
-    </row>
-    <row r="55" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="156" t="s">
+      <c r="F60" s="98"/>
+      <c r="P60" s="80"/>
+      <c r="Q60" s="80"/>
+      <c r="R60" s="80"/>
+      <c r="S60" s="80"/>
+    </row>
+    <row r="61" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="C55" s="129" t="s">
+      <c r="C61" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="99" t="s">
+      <c r="D61" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="F55" s="1"/>
-      <c r="P55" s="82"/>
-      <c r="Q55" s="82"/>
-      <c r="R55" s="82"/>
-      <c r="S55" s="82"/>
-    </row>
-    <row r="56" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B56" s="157"/>
-      <c r="C56" s="130">
+      <c r="F61" s="1"/>
+      <c r="P61" s="80"/>
+      <c r="Q61" s="80"/>
+      <c r="R61" s="80"/>
+      <c r="S61" s="80"/>
+    </row>
+    <row r="62" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B62" s="187"/>
+      <c r="C62" s="123">
         <v>0.67420000000000002</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D62" s="3">
         <v>0.83120000000000005</v>
       </c>
-      <c r="F56" s="1"/>
-      <c r="P56" s="82"/>
-      <c r="Q56" s="82"/>
-      <c r="R56" s="82"/>
-      <c r="S56" s="82"/>
-    </row>
-    <row r="57" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="157"/>
-      <c r="C57" s="130">
+      <c r="F62" s="1"/>
+      <c r="P62" s="80"/>
+      <c r="Q62" s="80"/>
+      <c r="R62" s="80"/>
+      <c r="S62" s="80"/>
+    </row>
+    <row r="63" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="187"/>
+      <c r="C63" s="123">
         <v>0.67449999999999999</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D63" s="3">
         <v>0.83130000000000004</v>
       </c>
-      <c r="F57" s="1"/>
-      <c r="P57" s="82"/>
-      <c r="Q57" s="82"/>
-      <c r="R57" s="82"/>
-      <c r="S57" s="82"/>
-    </row>
-    <row r="58" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="157"/>
-      <c r="C58" s="130">
+      <c r="F63" s="1"/>
+      <c r="P63" s="80"/>
+      <c r="Q63" s="80"/>
+      <c r="R63" s="80"/>
+      <c r="S63" s="80"/>
+    </row>
+    <row r="64" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="187"/>
+      <c r="C64" s="123">
         <v>0.67430000000000001</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D64" s="3">
         <v>0.83089999999999997</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="10" t="s">
+      <c r="F64" s="1"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="L58" s="38" t="s">
+      <c r="L64" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="P58" s="82"/>
-      <c r="Q58" s="82"/>
-      <c r="R58" s="82"/>
-      <c r="S58" s="82"/>
-    </row>
-    <row r="59" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="157"/>
-      <c r="C59" s="130">
+      <c r="P64" s="80"/>
+      <c r="Q64" s="80"/>
+      <c r="R64" s="80"/>
+      <c r="S64" s="80"/>
+    </row>
+    <row r="65" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="187"/>
+      <c r="C65" s="123">
         <v>0.6744</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D65" s="3">
         <v>0.8306</v>
       </c>
-      <c r="F59" s="1"/>
-      <c r="H59" s="159" t="s">
+      <c r="F65" s="1"/>
+      <c r="H65" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="I59" s="160"/>
-      <c r="J59" s="161"/>
-      <c r="K59" s="19">
+      <c r="I65" s="190"/>
+      <c r="J65" s="191"/>
+      <c r="K65" s="100">
         <f>'Facteurs correctifs'!C4*'Facteurs correctifs'!C26*'Facteurs correctifs'!C27</f>
-        <v>1.0119457606147688</v>
-      </c>
-      <c r="L59" s="39">
+        <v>1.0121458883237797</v>
+      </c>
+      <c r="L65" s="99">
         <f>'Facteurs correctifs'!C4*'Facteurs correctifs'!G26*'Facteurs correctifs'!G27</f>
         <v>1.0144155079597512</v>
       </c>
-      <c r="P59" s="82"/>
-      <c r="Q59" s="82"/>
-      <c r="R59" s="82"/>
-      <c r="S59" s="82"/>
-    </row>
-    <row r="60" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B60" s="157"/>
-      <c r="C60" s="130">
+      <c r="P65" s="80"/>
+      <c r="Q65" s="80"/>
+      <c r="R65" s="80"/>
+      <c r="S65" s="80"/>
+    </row>
+    <row r="66" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B66" s="187"/>
+      <c r="C66" s="123">
         <v>0.67520000000000002</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D66" s="3">
         <v>0.83079999999999998</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="P60" s="82"/>
-      <c r="Q60" s="82"/>
-      <c r="R60" s="82"/>
-      <c r="S60" s="82"/>
-    </row>
-    <row r="61" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B61" s="157"/>
-      <c r="C61" s="130">
+      <c r="F66" s="1"/>
+      <c r="P66" s="80"/>
+      <c r="Q66" s="80"/>
+      <c r="R66" s="80"/>
+      <c r="S66" s="80"/>
+    </row>
+    <row r="67" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="187"/>
+      <c r="C67" s="123">
         <v>0.67469999999999997</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D67" s="3">
         <v>0.83089999999999997</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="P61" s="82"/>
-      <c r="Q61" s="82"/>
-      <c r="R61" s="82"/>
-      <c r="S61" s="82"/>
-    </row>
-    <row r="62" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B62" s="157"/>
-      <c r="C62" s="130">
+      <c r="F67" s="1"/>
+      <c r="P67" s="80"/>
+      <c r="Q67" s="80"/>
+      <c r="R67" s="80"/>
+      <c r="S67" s="80"/>
+    </row>
+    <row r="68" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="187"/>
+      <c r="C68" s="123">
         <v>0.67490000000000006</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D68" s="3">
         <v>0.83130000000000004</v>
       </c>
-      <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B63" s="157"/>
-      <c r="C63" s="130">
+      <c r="F68" s="1"/>
+      <c r="I68" s="179" t="s">
+        <v>55</v>
+      </c>
+      <c r="J68" s="180"/>
+      <c r="K68" s="179" t="s">
+        <v>71</v>
+      </c>
+      <c r="L68" s="180"/>
+    </row>
+    <row r="69" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="187"/>
+      <c r="C69" s="123">
         <v>0.67520000000000002</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D69" s="3">
         <v>0.83099999999999996</v>
       </c>
-      <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B64" s="157"/>
-      <c r="C64" s="130">
+      <c r="F69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="132" t="s">
+        <v>0</v>
+      </c>
+      <c r="J69" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K69" s="133" t="s">
+        <v>0</v>
+      </c>
+      <c r="L69" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B70" s="187"/>
+      <c r="C70" s="123">
         <v>0.67569999999999997</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D70" s="3">
         <v>0.83160000000000001</v>
       </c>
-      <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="158"/>
-      <c r="C65" s="130">
+      <c r="F70" s="1"/>
+      <c r="H70" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="I70" s="144">
+        <f>STDEV(C6:C15)/C16*100</f>
+        <v>9.0540854652879851E-2</v>
+      </c>
+      <c r="J70" s="112">
+        <f>STDEV(E6:E15)/E16*100</f>
+        <v>4.1252722600962785E-2</v>
+      </c>
+      <c r="K70" s="145">
+        <f>C73/C72*100</f>
+        <v>0.12501544591463479</v>
+      </c>
+      <c r="L70" s="112">
+        <f>D73/D72*100</f>
+        <v>3.5331882282566611E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="188"/>
+      <c r="C71" s="123">
         <v>0.67700000000000005</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D71" s="3">
         <v>0.83120000000000005</v>
       </c>
-      <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B66" s="42" t="s">
+      <c r="F71" s="1"/>
+      <c r="H71" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="I71" s="146">
+        <f>'Facteurs correctifs'!F34/'Facteurs correctifs'!C26*100</f>
+        <v>0.11030036473487881</v>
+      </c>
+      <c r="J71" s="66">
+        <f>'Facteurs correctifs'!G34/'Facteurs correctifs'!C26*100</f>
+        <v>0.10844632462624132</v>
+      </c>
+      <c r="K71" s="147">
+        <f>'Facteurs correctifs'!H34/'Facteurs correctifs'!C26*100</f>
+        <v>5.8439360362767652E-2</v>
+      </c>
+      <c r="L71" s="66">
+        <f>'Facteurs correctifs'!I34/'Facteurs correctifs'!G26*100</f>
+        <v>0.10065181608088607</v>
+      </c>
+    </row>
+    <row r="72" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B72" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="6">
-        <f>AVERAGE(C55:C65)</f>
+      <c r="C72" s="6">
+        <f>AVERAGE(C61:C71)</f>
         <v>0.67501</v>
       </c>
-      <c r="D66" s="2">
-        <f>AVERAGE(D55:D65)</f>
+      <c r="D72" s="2">
+        <f>AVERAGE(D61:D71)</f>
         <v>0.83108000000000004</v>
       </c>
-      <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="44" t="s">
+      <c r="F72" s="1"/>
+      <c r="H72" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="I72" s="146">
+        <f>'Facteurs correctifs'!F35/'Facteurs correctifs'!C27*100</f>
+        <v>7.9584884721818377E-2</v>
+      </c>
+      <c r="J72" s="66">
+        <f>'Facteurs correctifs'!G35/'Facteurs correctifs'!C27*100</f>
+        <v>7.968741114200914E-2</v>
+      </c>
+      <c r="K72" s="147">
+        <f>'Facteurs correctifs'!H35/'Facteurs correctifs'!C27*100</f>
+        <v>3.1789898729895322E-2</v>
+      </c>
+      <c r="L72" s="66">
+        <f>'Facteurs correctifs'!I35/'Facteurs correctifs'!G27*100</f>
+        <v>9.2578024464032252E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="C67" s="131">
-        <f>STDEV(C56:C65)</f>
+      <c r="C73" s="124">
+        <f>STDEV(C62:C71)</f>
         <v>8.4386676146837617E-4</v>
       </c>
-      <c r="D67" s="115">
-        <f>STDEV(D56:D65)</f>
+      <c r="D73" s="109">
+        <f>STDEV(D62:D71)</f>
         <v>2.9363620727395457E-4</v>
       </c>
-    </row>
-    <row r="68" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="162" t="s">
+      <c r="H73" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="I73" s="146">
+        <f>'Facteurs correctifs'!C36*100</f>
+        <v>0.27529622421882033</v>
+      </c>
+      <c r="J73" s="66">
+        <f>'Facteurs correctifs'!C36*100</f>
+        <v>0.27529622421882033</v>
+      </c>
+      <c r="K73" s="147">
+        <f>'Facteurs correctifs'!C36*100</f>
+        <v>0.27529622421882033</v>
+      </c>
+      <c r="L73" s="66">
+        <f>'Facteurs correctifs'!C36*100</f>
+        <v>0.27529622421882033</v>
+      </c>
+    </row>
+    <row r="74" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H74" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="I74" s="11">
+        <f>J5</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J74" s="3">
+        <f>J5</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K74" s="1">
+        <f>N5</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L74" s="3">
+        <f>J5</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="192" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="168"/>
-      <c r="D69" s="132" t="s">
+      <c r="C75" s="193"/>
+      <c r="D75" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="165" t="s">
+      <c r="E75" s="134" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B70" s="166" t="s">
+      <c r="H75" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="I75" s="11">
+        <v>1</v>
+      </c>
+      <c r="J75" s="3">
+        <v>1</v>
+      </c>
+      <c r="K75" s="1">
+        <v>1</v>
+      </c>
+      <c r="L75" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="42" t="s">
+      <c r="C76" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D70" s="118">
-        <f>C66*K59*M5*C22</f>
-        <v>1.5956179622524382</v>
-      </c>
-      <c r="E70" s="117">
-        <f>D66*L59*D22*M5</f>
+      <c r="D76" s="112">
+        <f>C72*K65*M5*C22</f>
+        <v>1.5959335200418678</v>
+      </c>
+      <c r="E76" s="111">
+        <f>D72*L65*D22*M5</f>
         <v>1.9300332490838961</v>
       </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B71" s="167"/>
-      <c r="C71" s="43" t="s">
+      <c r="H76" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="I76" s="148">
+        <f>SQRT((I70/100)^2+(I71/100)^2+(I72/100)^2+(I73/100)^2+(I74/100)^2+(I75/100)^2)*100</f>
+        <v>1.1853208771329582</v>
+      </c>
+      <c r="J76" s="150">
+        <f>SQRT((J70/100)^2+(J71/100)^2+(J72/100)^2+(J73/100)^2+(J74/100)^2+(J75/100)^2)*100</f>
+        <v>1.1824129934209056</v>
+      </c>
+      <c r="K76" s="149">
+        <f>SQRT((K70/100)^2+(K71/100)^2+(K72/100)^2+(K73/100)^2+(K74/100)^2+(K75/100)^2)*100</f>
+        <v>1.1825153822624213</v>
+      </c>
+      <c r="L76" s="150">
+        <f>SQRT((L70/100)^2+(L71/100)^2+(L72/100)^2+(L73/100)^2+(L74/100)^2+(L75/100)^2)*100</f>
+        <v>1.1824710701191854</v>
+      </c>
+    </row>
+    <row r="77" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="177"/>
+      <c r="C77" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D71" s="68">
+      <c r="D77" s="66">
         <v>1.589</v>
       </c>
-      <c r="E71" s="67">
+      <c r="E77" s="65">
         <v>1.907</v>
       </c>
-    </row>
-    <row r="72" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="158"/>
-      <c r="C72" s="44" t="s">
+      <c r="H77" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="I77" s="151">
+        <f>I76*2</f>
+        <v>2.3706417542659164</v>
+      </c>
+      <c r="J77" s="153">
+        <f>J76*2</f>
+        <v>2.3648259868418111</v>
+      </c>
+      <c r="K77" s="152">
+        <f>K76*2</f>
+        <v>2.3650307645248425</v>
+      </c>
+      <c r="L77" s="153">
+        <f>L76*2</f>
+        <v>2.3649421402383708</v>
+      </c>
+    </row>
+    <row r="78" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="177"/>
+      <c r="C78" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D72" s="62">
-        <f>(ABS(D70-D71)/D71*100)</f>
-        <v>0.41648598190297487</v>
-      </c>
-      <c r="E72" s="57">
-        <f>ABS(E70-E71)/E71*100</f>
+      <c r="D78" s="60">
+        <f>(ABS(D76-D77)/D77*100)</f>
+        <v>0.43634487362289925</v>
+      </c>
+      <c r="E78" s="55">
+        <f>ABS(E76-E77)/E77*100</f>
         <v>1.207826380906976</v>
       </c>
     </row>
-    <row r="73" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C74" s="132" t="s">
+    <row r="79" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="178"/>
+      <c r="C79" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="D79" s="156">
+        <f>ABS(D76-D26)/D26*100</f>
+        <v>8.3432867776990716E-2</v>
+      </c>
+      <c r="E79" s="157">
+        <f>ABS(E76-E26)/E26*100</f>
+        <v>0.135860105986011</v>
+      </c>
+    </row>
+    <row r="80" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C81" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="D74" s="120" t="s">
+      <c r="D81" s="114" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B75" s="104" t="s">
-        <v>58</v>
-      </c>
-      <c r="C75" s="117">
-        <f>D70*SQRT((STDEV(C56:C65)/C66)^2+(1/100)^2+'Facteurs correctifs'!C36^2+('Facteurs correctifs'!H34/'Facteurs correctifs'!G26)^2+('Facteurs correctifs'!H35/'Facteurs correctifs'!G27)^2+('Mesures Clinac 2'!N5/100)^2)</f>
-        <v>1.8868366820130867E-2</v>
-      </c>
-      <c r="D75" s="121">
-        <f>E70*SQRT((STDEV(D56:D65)/D66)^2+(1/100)^2+'Facteurs correctifs'!C36^2+('Facteurs correctifs'!I34/'Facteurs correctifs'!G26)^2+('Facteurs correctifs'!I35/'Facteurs correctifs'!G27)^2+('Mesures Clinac 2'!N5/100)^2)</f>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B82" s="102" t="s">
+        <v>57</v>
+      </c>
+      <c r="C82" s="111">
+        <f>D76*SQRT((STDEV(C62:C71)/C72)^2+(1/100)^2+'Facteurs correctifs'!C36^2+('Facteurs correctifs'!H34/'Facteurs correctifs'!G26)^2+('Facteurs correctifs'!H35/'Facteurs correctifs'!G27)^2+('Mesures Clinac 2'!N5/100)^2)</f>
+        <v>1.8872101016574362E-2</v>
+      </c>
+      <c r="D82" s="115">
+        <f>E76*SQRT((STDEV(D62:D71)/D72)^2+(1/100)^2+'Facteurs correctifs'!C36^2+('Facteurs correctifs'!I34/'Facteurs correctifs'!G26)^2+('Facteurs correctifs'!I35/'Facteurs correctifs'!G27)^2+('Mesures Clinac 2'!N5/100)^2)</f>
         <v>2.2822084814098434E-2</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B76" s="105" t="s">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B83" s="103" t="s">
+        <v>63</v>
+      </c>
+      <c r="C83" s="65">
+        <f>C82*2</f>
+        <v>3.7744202033148724E-2</v>
+      </c>
+      <c r="D83" s="66">
+        <f>D82*2</f>
+        <v>4.5644169628196868E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="C76" s="67">
-        <f>C75*2</f>
-        <v>3.7736733640261734E-2</v>
-      </c>
-      <c r="D76" s="68">
-        <f>D75*2</f>
-        <v>4.5644169628196868E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="106" t="s">
-        <v>65</v>
-      </c>
-      <c r="C77" s="57">
-        <f>C76/D70*100</f>
-        <v>2.3650231153697372</v>
-      </c>
-      <c r="D77" s="62">
-        <f>D76/E70*100</f>
+      <c r="C84" s="55">
+        <f>C83/D76*100</f>
+        <v>2.3650234523652678</v>
+      </c>
+      <c r="D84" s="68">
+        <f>D83/E76*100</f>
         <v>2.3649421402383712</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:B72"/>
+  <mergeCells count="26">
+    <mergeCell ref="N43:P43"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="B55:B65"/>
-    <mergeCell ref="H59:J59"/>
+    <mergeCell ref="B57:L57"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="B37:B47"/>
@@ -6417,13 +6996,19 @@
     <mergeCell ref="K36:L36"/>
     <mergeCell ref="H37:H47"/>
     <mergeCell ref="B34:L34"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B5:B15"/>
     <mergeCell ref="H12:J12"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B61:B71"/>
+    <mergeCell ref="H65:J65"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6434,7 +7019,7 @@
   <dimension ref="B1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6443,8 +7028,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="109" t="s">
-        <v>62</v>
+      <c r="B1" s="107" t="s">
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -6458,16 +7043,16 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49">
+        <v>59</v>
+      </c>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47">
         <v>1017</v>
       </c>
-      <c r="I2" s="49"/>
+      <c r="I2" s="47"/>
       <c r="J2" s="2">
         <v>1013.25</v>
       </c>
@@ -6502,7 +7087,7 @@
         <v>38.72</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="4">
         <f>(J2*(H3+273.15))/((J3+273.15)*H2)</f>
@@ -6601,31 +7186,31 @@
     </row>
     <row r="13" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
-      <c r="C13" s="107">
+      <c r="C13" s="105">
         <f>AVERAGE(C3:C12)</f>
         <v>32.820999999999998</v>
       </c>
-      <c r="D13" s="108">
+      <c r="D13" s="106">
         <f>AVERAGE(D3:D12)</f>
         <v>38.729000000000006</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16">
         <f>C13*H4*'Facteurs correctifs'!C14*'Facteurs correctifs'!C15*'Mesures Clinac 2'!C22*'Mesures Clinac 2'!I5</f>
-        <v>1.7605729058811133</v>
+        <v>1.7635312994869627</v>
       </c>
       <c r="D16">
         <f>D13*H4*'Facteurs correctifs'!G14*'Facteurs correctifs'!G15*'Mesures Clinac 2'!I5*'Mesures Clinac 2'!D22</f>
-        <v>2.0412422773039065</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="109" t="s">
-        <v>63</v>
+        <v>2.0446722960671129</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="107" t="s">
+        <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
@@ -6634,18 +7219,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="E20" s="161" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>1</v>
       </c>
@@ -6656,7 +7244,7 @@
         <v>36.65</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>2</v>
       </c>
@@ -6667,7 +7255,7 @@
         <v>36.590000000000003</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>3</v>
       </c>
@@ -6678,7 +7266,7 @@
         <v>36.58</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>4</v>
       </c>
@@ -6689,7 +7277,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>5</v>
       </c>
@@ -6700,38 +7288,38 @@
         <v>36.619999999999997</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="107">
+      <c r="C26" s="105">
         <f>AVERAGE(C21:C25)</f>
         <v>29.686</v>
       </c>
-      <c r="D26" s="107">
+      <c r="D26" s="196">
         <f>AVERAGE(D21:D25)</f>
         <v>36.608000000000004</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
     </row>
   </sheetData>
@@ -6756,13 +7344,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>48</v>
       </c>
       <c r="D1" s="13"/>
@@ -6771,279 +7359,279 @@
       <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="25">
+      <c r="A2" s="24">
         <v>0</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2" s="53">
         <v>15.52</v>
       </c>
-      <c r="C2" s="71">
+      <c r="C2" s="69">
         <v>8.3089999999999993</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="86">
+      <c r="A3" s="84">
         <v>1</v>
       </c>
-      <c r="B3" s="56">
+      <c r="B3" s="54">
         <v>35.94</v>
       </c>
-      <c r="C3" s="85">
+      <c r="C3" s="83">
         <v>28.64</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="86">
+      <c r="A4" s="84">
         <v>2</v>
       </c>
-      <c r="B4" s="56">
+      <c r="B4" s="54">
         <v>36.83</v>
       </c>
-      <c r="C4" s="85">
+      <c r="C4" s="83">
         <v>36.19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="86">
+      <c r="A5" s="84">
         <v>3</v>
       </c>
-      <c r="B5" s="56">
+      <c r="B5" s="54">
         <v>35.299999999999997</v>
       </c>
-      <c r="C5" s="85">
+      <c r="C5" s="83">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="86">
+      <c r="A6" s="84">
         <v>4</v>
       </c>
-      <c r="B6" s="56">
+      <c r="B6" s="54">
         <v>33.729999999999997</v>
       </c>
-      <c r="C6" s="85">
+      <c r="C6" s="83">
         <v>37.78</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="86">
+      <c r="A7" s="84">
         <v>5</v>
       </c>
-      <c r="B7" s="56">
+      <c r="B7" s="54">
         <v>32.15</v>
       </c>
-      <c r="C7" s="85">
+      <c r="C7" s="83">
         <v>36.76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="86">
+      <c r="A8" s="84">
         <v>6</v>
       </c>
-      <c r="B8" s="56">
+      <c r="B8" s="54">
         <v>30.6</v>
       </c>
-      <c r="C8" s="85">
+      <c r="C8" s="83">
         <v>35.51</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="86">
+      <c r="A9" s="84">
         <v>7</v>
       </c>
-      <c r="B9" s="56">
+      <c r="B9" s="54">
         <v>29.05</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="83">
         <v>34.19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="86">
+      <c r="A10" s="84">
         <v>8</v>
       </c>
-      <c r="B10" s="56">
+      <c r="B10" s="54">
         <v>27.56</v>
       </c>
-      <c r="C10" s="85">
+      <c r="C10" s="83">
         <v>32.89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="86">
+      <c r="A11" s="84">
         <v>9</v>
       </c>
-      <c r="B11" s="56">
+      <c r="B11" s="54">
         <v>26.14</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="83">
         <v>31.58</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="86">
+      <c r="A12" s="84">
         <v>10</v>
       </c>
-      <c r="B12" s="56">
+      <c r="B12" s="54">
         <v>24.76</v>
       </c>
-      <c r="C12" s="85">
+      <c r="C12" s="83">
         <v>30.35</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="86">
+      <c r="A13" s="84">
         <v>11</v>
       </c>
-      <c r="B13" s="56">
+      <c r="B13" s="54">
         <v>23.45</v>
       </c>
-      <c r="C13" s="85">
+      <c r="C13" s="83">
         <v>29.13</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="86">
+      <c r="A14" s="84">
         <v>12</v>
       </c>
-      <c r="B14" s="56">
+      <c r="B14" s="54">
         <v>22.2</v>
       </c>
-      <c r="C14" s="85">
+      <c r="C14" s="83">
         <v>27.99</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="86">
+      <c r="A15" s="84">
         <v>13</v>
       </c>
-      <c r="B15" s="56">
+      <c r="B15" s="54">
         <v>20.96</v>
       </c>
-      <c r="C15" s="85">
+      <c r="C15" s="83">
         <v>26.84</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="86">
+      <c r="A16" s="84">
         <v>14</v>
       </c>
-      <c r="B16" s="56">
+      <c r="B16" s="54">
         <v>19.84</v>
       </c>
-      <c r="C16" s="85">
+      <c r="C16" s="83">
         <v>25.78</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="86">
+      <c r="A17" s="84">
         <v>15</v>
       </c>
-      <c r="B17" s="56">
+      <c r="B17" s="54">
         <v>18.73</v>
       </c>
-      <c r="C17" s="85">
+      <c r="C17" s="83">
         <v>24.73</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="86">
+      <c r="A18" s="84">
         <v>16</v>
       </c>
-      <c r="B18" s="56">
+      <c r="B18" s="54">
         <v>17.73</v>
       </c>
-      <c r="C18" s="85">
+      <c r="C18" s="83">
         <v>23.75</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="86">
+      <c r="A19" s="84">
         <v>17</v>
       </c>
-      <c r="B19" s="56">
+      <c r="B19" s="54">
         <v>16.739999999999998</v>
       </c>
-      <c r="C19" s="85">
+      <c r="C19" s="83">
         <v>22.78</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="86">
+      <c r="A20" s="84">
         <v>18</v>
       </c>
-      <c r="B20" s="56">
+      <c r="B20" s="54">
         <v>15.83</v>
       </c>
-      <c r="C20" s="85">
+      <c r="C20" s="83">
         <v>21.87</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="86">
+      <c r="A21" s="84">
         <v>19</v>
       </c>
-      <c r="B21" s="56">
+      <c r="B21" s="54">
         <v>14.93</v>
       </c>
-      <c r="C21" s="85">
+      <c r="C21" s="83">
         <v>20.99</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="86">
+      <c r="A22" s="84">
         <v>20</v>
       </c>
-      <c r="B22" s="56">
+      <c r="B22" s="54">
         <v>14.13</v>
       </c>
-      <c r="C22" s="85">
+      <c r="C22" s="83">
         <v>20.149999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="86">
+      <c r="A23" s="84">
         <v>21</v>
       </c>
-      <c r="B23" s="56">
+      <c r="B23" s="54">
         <v>13.33</v>
       </c>
-      <c r="C23" s="85">
+      <c r="C23" s="83">
         <v>19.309999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="86">
+      <c r="A24" s="84">
         <v>22</v>
       </c>
-      <c r="B24" s="56">
+      <c r="B24" s="54">
         <v>12.6</v>
       </c>
-      <c r="C24" s="85">
+      <c r="C24" s="83">
         <v>18.54</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26">
+      <c r="A25" s="25">
         <v>23</v>
       </c>
-      <c r="B25" s="89">
+      <c r="B25" s="87">
         <v>11.9</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="60">
         <v>17.78</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J27" s="30" t="s">
+      <c r="J27" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="87">
+      <c r="K27" s="85">
         <f>B22/B12</f>
         <v>0.57067851373182554</v>
       </c>
-      <c r="L27" s="88">
+      <c r="L27" s="86">
         <f>C22/C12</f>
         <v>0.66392092257001645</v>
       </c>
@@ -7052,48 +7640,48 @@
       <c r="J28" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="83">
+      <c r="K28" s="81">
         <f>1.2661*K27-0.0595</f>
         <v>0.66303606623586431</v>
       </c>
-      <c r="L28" s="84">
+      <c r="L28" s="82">
         <f>1.2661*L27-0.0595</f>
         <v>0.78109028006589787</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J29" s="90" t="s">
+      <c r="J29" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="K29" s="91">
+      <c r="K29" s="89">
         <v>0.56999999999999995</v>
       </c>
-      <c r="L29" s="92">
+      <c r="L29" s="90">
         <v>0.66</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J30" s="93" t="s">
+      <c r="J30" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="K30" s="94">
+      <c r="K30" s="92">
         <f>ABS(K29-K27)/K29*100</f>
         <v>0.11903749681150735</v>
       </c>
-      <c r="L30" s="95">
+      <c r="L30" s="93">
         <f>ABS(L29-L27)/L29*100</f>
         <v>0.59407917727521453</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J31" s="96" t="s">
+      <c r="J31" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="K31" s="97">
+      <c r="K31" s="95">
         <f>ABS(K28-'Mesures Clinac 2'!C19)/'Mesures Clinac 2'!C19*100</f>
         <v>0.14517074761080226</v>
       </c>
-      <c r="L31" s="98">
+      <c r="L31" s="96">
         <f>ABS(L28-'Mesures Clinac 2'!D19)/'Mesures Clinac 2'!D19*100</f>
         <v>1.155954749012047E-2</v>
       </c>
@@ -7115,288 +7703,288 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="108" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="110" t="s">
+      <c r="C1" s="108" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="110">
+      <c r="A2" s="108">
         <v>0</v>
       </c>
-      <c r="B2" s="110">
+      <c r="B2" s="108">
         <v>15.86</v>
       </c>
-      <c r="C2" s="110">
+      <c r="C2" s="108">
         <v>10.119999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="110">
+      <c r="A3" s="108">
         <v>0.2</v>
       </c>
-      <c r="B3" s="110">
+      <c r="B3" s="108">
         <v>17.3</v>
       </c>
-      <c r="C3" s="110">
+      <c r="C3" s="108">
         <v>11.03</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="110">
+      <c r="A4" s="108">
         <v>0.4</v>
       </c>
-      <c r="B4" s="110">
+      <c r="B4" s="108">
         <v>20.75</v>
       </c>
-      <c r="C4" s="110">
+      <c r="C4" s="108">
         <v>13.34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="110">
+      <c r="A5" s="108">
         <v>0.6</v>
       </c>
-      <c r="B5" s="110">
+      <c r="B5" s="108">
         <v>31.7</v>
       </c>
-      <c r="C5" s="110">
+      <c r="C5" s="108">
         <v>22.15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="110">
+      <c r="A6" s="108">
         <v>0.8</v>
       </c>
-      <c r="B6" s="110">
+      <c r="B6" s="108">
         <v>34.65</v>
       </c>
-      <c r="C6" s="110">
+      <c r="C6" s="108">
         <v>26.05</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="110">
+      <c r="A7" s="108">
         <v>1</v>
       </c>
-      <c r="B7" s="110">
+      <c r="B7" s="108">
         <v>36.229999999999997</v>
       </c>
-      <c r="C7" s="110">
+      <c r="C7" s="108">
         <v>29.11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="110">
+      <c r="A8" s="108">
         <v>1.2</v>
       </c>
-      <c r="B8" s="110">
+      <c r="B8" s="108">
         <v>36.93</v>
       </c>
-      <c r="C8" s="110">
+      <c r="C8" s="108">
         <v>31.33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="110">
+      <c r="A9" s="108">
         <v>1.4</v>
       </c>
-      <c r="B9" s="110">
+      <c r="B9" s="108">
         <v>37.229999999999997</v>
       </c>
-      <c r="C9" s="110">
+      <c r="C9" s="108">
         <v>33.14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="110">
+      <c r="A10" s="108">
         <v>1.6</v>
       </c>
-      <c r="B10" s="110">
+      <c r="B10" s="108">
         <v>37.229999999999997</v>
       </c>
-      <c r="C10" s="110">
+      <c r="C10" s="108">
         <v>34.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="110">
+      <c r="A11" s="108">
         <v>1.8</v>
       </c>
-      <c r="B11" s="110">
+      <c r="B11" s="108">
         <v>37.08</v>
       </c>
-      <c r="C11" s="110">
+      <c r="C11" s="108">
         <v>35.57</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="110">
+      <c r="A12" s="108">
         <v>2</v>
       </c>
-      <c r="B12" s="110">
+      <c r="B12" s="108">
         <v>36.909999999999997</v>
       </c>
-      <c r="C12" s="110">
+      <c r="C12" s="108">
         <v>36.340000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="110">
+      <c r="A13" s="108">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B13" s="110">
+      <c r="B13" s="108">
         <v>36.65</v>
       </c>
-      <c r="C13" s="110">
+      <c r="C13" s="108">
         <v>36.979999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="110">
+      <c r="A14" s="108">
         <v>2.4</v>
       </c>
-      <c r="B14" s="110">
+      <c r="B14" s="108">
         <v>36.299999999999997</v>
       </c>
-      <c r="C14" s="110">
+      <c r="C14" s="108">
         <v>37.4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="110">
+      <c r="A15" s="108">
         <v>2.6</v>
       </c>
-      <c r="B15" s="110">
+      <c r="B15" s="108">
         <v>35.979999999999997</v>
       </c>
-      <c r="C15" s="110">
+      <c r="C15" s="108">
         <v>37.770000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="110">
+      <c r="A16" s="108">
         <v>2.8</v>
       </c>
-      <c r="B16" s="110">
+      <c r="B16" s="108">
         <v>35.69</v>
       </c>
-      <c r="C16" s="110">
+      <c r="C16" s="108">
         <v>37.93</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="110">
+      <c r="A17" s="108">
         <v>3</v>
       </c>
-      <c r="B17" s="110">
+      <c r="B17" s="108">
         <v>35.35</v>
       </c>
-      <c r="C17" s="110">
+      <c r="C17" s="108">
         <v>38.090000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="110">
+      <c r="A18" s="108">
         <v>3.5</v>
       </c>
-      <c r="B18" s="110">
+      <c r="B18" s="108">
         <v>34.56</v>
       </c>
-      <c r="C18" s="110">
+      <c r="C18" s="108">
         <v>38.06</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="110">
+      <c r="A19" s="108">
         <v>4</v>
       </c>
-      <c r="B19" s="110">
+      <c r="B19" s="108">
         <v>33.76</v>
       </c>
-      <c r="C19" s="110">
+      <c r="C19" s="108">
         <v>37.81</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="110">
+      <c r="A20" s="108">
         <v>6</v>
       </c>
-      <c r="B20" s="110">
+      <c r="B20" s="108">
         <v>30.63</v>
       </c>
-      <c r="C20" s="110">
+      <c r="C20" s="108">
         <v>35.49</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="110">
+      <c r="A21" s="108">
         <v>9</v>
       </c>
-      <c r="B21" s="110">
+      <c r="B21" s="108">
         <v>26.15</v>
       </c>
-      <c r="C21" s="110">
+      <c r="C21" s="108">
         <v>31.62</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="110">
+      <c r="A22" s="108">
         <v>12</v>
       </c>
-      <c r="B22" s="110">
+      <c r="B22" s="108">
         <v>22.21</v>
       </c>
-      <c r="C22" s="110">
+      <c r="C22" s="108">
         <v>27.97</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="110">
+      <c r="A23" s="108">
         <v>15</v>
       </c>
-      <c r="B23" s="110">
+      <c r="B23" s="108">
         <v>18.739999999999998</v>
       </c>
-      <c r="C23" s="110">
+      <c r="C23" s="108">
         <v>24.75</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="110">
+      <c r="A24" s="108">
         <v>18</v>
       </c>
-      <c r="B24" s="110">
+      <c r="B24" s="108">
         <v>15.86</v>
       </c>
-      <c r="C24" s="110">
+      <c r="C24" s="108">
         <v>21.86</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="110">
+      <c r="A25" s="108">
         <v>21</v>
       </c>
-      <c r="B25" s="110">
+      <c r="B25" s="108">
         <v>13.35</v>
       </c>
-      <c r="C25" s="110">
+      <c r="C25" s="108">
         <v>19.34</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="110">
+      <c r="A26" s="108">
         <v>23</v>
       </c>
-      <c r="B26" s="110">
+      <c r="B26" s="108">
         <v>11.24</v>
       </c>
-      <c r="C26" s="110">
+      <c r="C26" s="108">
         <v>17.07</v>
       </c>
     </row>

</xml_diff>